<commit_message>
teamrankings scrape and merge work, except overrides
</commit_message>
<xml_diff>
--- a/data/merge.xlsx
+++ b/data/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="716">
   <si>
     <t>Index</t>
   </si>
@@ -1408,360 +1408,360 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>NC State</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>W Virginia</t>
+  </si>
+  <si>
     <t>W Kentucky</t>
   </si>
   <si>
-    <t>NC State</t>
-  </si>
-  <si>
-    <t>Liberty</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Florida St</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Kansas St</t>
+  </si>
+  <si>
+    <t>U Mass</t>
+  </si>
+  <si>
+    <t>Oregon St</t>
+  </si>
+  <si>
+    <t>Georgia St</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>S Florida</t>
+  </si>
+  <si>
+    <t>Fresno St</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>N Carolina</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>Penn St</t>
+  </si>
+  <si>
+    <t>Akron</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>VA Tech</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Wake Forest</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>N Mex State</t>
+  </si>
+  <si>
+    <t>Wash State</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>San Diego St</t>
+  </si>
+  <si>
+    <t>App State</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Colorado St</t>
   </si>
   <si>
     <t>Virginia</t>
   </si>
   <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Florida St</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Kansas St</t>
-  </si>
-  <si>
-    <t>U Mass</t>
-  </si>
-  <si>
-    <t>Oregon St</t>
-  </si>
-  <si>
-    <t>Georgia St</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>Fresno St</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>N Carolina</t>
-  </si>
-  <si>
-    <t>Indiana</t>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Miss State</t>
+  </si>
+  <si>
+    <t>GA Tech</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>UL Monroe</t>
+  </si>
+  <si>
+    <t>LA Tech</t>
+  </si>
+  <si>
+    <t>S Methodist</t>
+  </si>
+  <si>
+    <t>James Mad</t>
+  </si>
+  <si>
+    <t>E Michigan</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Oklahoma St</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Ball St</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>TX Christian</t>
+  </si>
+  <si>
+    <t>Middle Tenn</t>
+  </si>
+  <si>
+    <t>Kent St</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>S Alabama</t>
+  </si>
+  <si>
+    <t>Sam Hous St</t>
+  </si>
+  <si>
+    <t>Notre Dame</t>
+  </si>
+  <si>
+    <t>Coastal Car</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Texas St</t>
   </si>
   <si>
     <t>Alabama</t>
   </si>
   <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Cincinnati</t>
-  </si>
-  <si>
-    <t>Penn St</t>
-  </si>
-  <si>
-    <t>Akron</t>
-  </si>
-  <si>
-    <t>Duke</t>
-  </si>
-  <si>
-    <t>LA Tech</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Wake Forest</t>
-  </si>
-  <si>
-    <t>N Mex State</t>
-  </si>
-  <si>
-    <t>Wash State</t>
-  </si>
-  <si>
-    <t>Louisville</t>
-  </si>
-  <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
-    <t>San Diego St</t>
-  </si>
-  <si>
-    <t>App State</t>
-  </si>
-  <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Colorado St</t>
-  </si>
-  <si>
-    <t>W Virginia</t>
-  </si>
-  <si>
-    <t>Army</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Miss State</t>
-  </si>
-  <si>
-    <t>S Methodist</t>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>Fla Atlantic</t>
+  </si>
+  <si>
+    <t>Bowling Grn</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>N Illinois</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>Texas Tech</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Michigan St</t>
+  </si>
+  <si>
+    <t>Boston Col</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
   </si>
   <si>
     <t>Missouri</t>
   </si>
   <si>
-    <t>GA Tech</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>UL Monroe</t>
-  </si>
-  <si>
-    <t>Sam Hous St</t>
-  </si>
-  <si>
-    <t>James Mad</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>E Michigan</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Oklahoma St</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Ball St</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>TX Christian</t>
-  </si>
-  <si>
-    <t>Middle Tenn</t>
-  </si>
-  <si>
-    <t>Kent St</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Temple</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Stanford</t>
-  </si>
-  <si>
-    <t>Notre Dame</t>
-  </si>
-  <si>
-    <t>Coastal Car</t>
-  </si>
-  <si>
-    <t>Syracuse</t>
-  </si>
-  <si>
-    <t>Texas St</t>
-  </si>
-  <si>
-    <t>S Alabama</t>
-  </si>
-  <si>
-    <t>Auburn</t>
-  </si>
-  <si>
-    <t>Fla Atlantic</t>
-  </si>
-  <si>
-    <t>Bowling Grn</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
+    <t>Purdue</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M</t>
+  </si>
+  <si>
+    <t>Jksnville St</t>
+  </si>
+  <si>
+    <t>Old Dominion</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Central Mich</t>
   </si>
   <si>
     <t>Illinois</t>
   </si>
   <si>
-    <t>Northwestern</t>
-  </si>
-  <si>
-    <t>Texas Tech</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Michigan St</t>
-  </si>
-  <si>
-    <t>Boston Col</t>
+    <t>TX El Paso</t>
   </si>
   <si>
     <t>Ohio St</t>
   </si>
   <si>
-    <t>Buffalo</t>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>E Carolina</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Iowa St</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Arizona</t>
   </si>
   <si>
     <t>Mississippi</t>
   </si>
   <si>
-    <t>Purdue</t>
-  </si>
-  <si>
-    <t>Texas A&amp;M</t>
-  </si>
-  <si>
-    <t>Jksnville St</t>
-  </si>
-  <si>
-    <t>VA Tech</t>
-  </si>
-  <si>
-    <t>Old Dominion</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Central Mich</t>
-  </si>
-  <si>
-    <t>TX El Paso</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
+    <t>Arkansas St</t>
+  </si>
+  <si>
+    <t>W Michigan</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>GA Southern</t>
+  </si>
+  <si>
+    <t>Baylor</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Boise St</t>
+  </si>
+  <si>
+    <t>S Mississippi</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Arizona St</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>North Texas</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Tulane</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>Florida Intl</t>
   </si>
   <si>
     <t>California</t>
   </si>
   <si>
-    <t>W Michigan</t>
-  </si>
-  <si>
-    <t>Iowa St</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>S Mississippi</t>
-  </si>
-  <si>
-    <t>Arkansas St</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Toledo</t>
-  </si>
-  <si>
-    <t>Tulsa</t>
-  </si>
-  <si>
-    <t>GA Southern</t>
-  </si>
-  <si>
-    <t>Baylor</t>
-  </si>
-  <si>
-    <t>Troy</t>
-  </si>
-  <si>
-    <t>Boise St</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Arizona St</t>
-  </si>
-  <si>
-    <t>Marshall</t>
-  </si>
-  <si>
-    <t>North Texas</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>Tulane</t>
-  </si>
-  <si>
-    <t>Navy</t>
-  </si>
-  <si>
-    <t>Florida Intl</t>
-  </si>
-  <si>
-    <t>E Carolina</t>
-  </si>
-  <si>
-    <t>S Florida</t>
-  </si>
-  <si>
     <t>Rutgers</t>
   </si>
   <si>
     <t>S Carolina</t>
   </si>
   <si>
-    <t>N Illinois</t>
-  </si>
-  <si>
     <t>Air Force</t>
   </si>
   <si>
@@ -1783,652 +1783,385 @@
     <t>Iowa</t>
   </si>
   <si>
-    <t>MONTANA STATE</t>
-  </si>
-  <si>
-    <t>LAWRENCE TECH (MI)</t>
-  </si>
-  <si>
-    <t>OTTAWA-KANSAS</t>
-  </si>
-  <si>
-    <t>BETHUNE-COOKMAN</t>
-  </si>
-  <si>
-    <t>CHARLESTON SOUTHERN</t>
-  </si>
-  <si>
-    <t>VALLEY CITY STATE</t>
-  </si>
-  <si>
-    <t>S.F.AUSTIN</t>
-  </si>
-  <si>
-    <t>PRINCETON</t>
-  </si>
-  <si>
-    <t>CENTRAL METHODIST</t>
-  </si>
-  <si>
-    <t>STETSON</t>
-  </si>
-  <si>
-    <t>NORTHERN COLORADO</t>
-  </si>
-  <si>
-    <t>L.I.U. - POST</t>
-  </si>
-  <si>
-    <t>RICHMOND</t>
-  </si>
-  <si>
-    <t>HAMPTON</t>
-  </si>
-  <si>
-    <t>GEORGETOWN-KY.</t>
-  </si>
-  <si>
-    <t>FORDHAM</t>
-  </si>
-  <si>
-    <t>LINDENWOOD - MO</t>
-  </si>
-  <si>
-    <t>DORDT</t>
-  </si>
-  <si>
-    <t>DOANE</t>
-  </si>
-  <si>
-    <t>S W ASSMEMBLY OF GOD</t>
-  </si>
-  <si>
-    <t>IDAHO STATE</t>
-  </si>
-  <si>
-    <t>FRIENDS</t>
-  </si>
-  <si>
-    <t>KANSAS WESLEYAN</t>
-  </si>
-  <si>
-    <t>HOUSTON CHRISTIAN</t>
-  </si>
-  <si>
-    <t>SOUTH EASTERN MISSOURI</t>
-  </si>
-  <si>
-    <t>MOREHEAD STATE</t>
-  </si>
-  <si>
-    <t>BETHEL-TN.</t>
-  </si>
-  <si>
-    <t>NORFOLK STATE</t>
-  </si>
-  <si>
-    <t>MID-AMERICA NAZARENE</t>
-  </si>
-  <si>
-    <t>NORTHWESTERN-IOWA</t>
-  </si>
-  <si>
-    <t>SOUTHERN ILLINOIS</t>
-  </si>
-  <si>
-    <t>NORTHERN IOWA</t>
-  </si>
-  <si>
-    <t>NORTHWESTERN STATE-LA</t>
-  </si>
-  <si>
-    <t>THOMAS - GA</t>
-  </si>
-  <si>
-    <t>CAMPBELLSVILLE</t>
-  </si>
-  <si>
-    <t>ST.MARY-KANSAS</t>
-  </si>
-  <si>
-    <t>NORTH AMERICAN - TEXAS</t>
-  </si>
-  <si>
-    <t>NORTH CAROLINA A&amp;T</t>
-  </si>
-  <si>
-    <t>MISSOURI STATE</t>
-  </si>
-  <si>
-    <t>CLARKE - IOWA</t>
-  </si>
-  <si>
-    <t>JUDSON</t>
-  </si>
-  <si>
-    <t>MARIAN - INDIANA</t>
-  </si>
-  <si>
-    <t>PRAIRIE VIEW A&amp;M</t>
-  </si>
-  <si>
-    <t>ALABAMA A&amp;M</t>
-  </si>
-  <si>
-    <t>SOUTHEASTERN -FLA</t>
-  </si>
-  <si>
-    <t>ST.AMBROSE</t>
-  </si>
-  <si>
-    <t>CENTRAL CONNECTICUT ST.</t>
-  </si>
-  <si>
-    <t>INDIANA WESLEYAN</t>
-  </si>
-  <si>
-    <t>PERU STATE</t>
-  </si>
-  <si>
-    <t>BROWN</t>
-  </si>
-  <si>
-    <t>BUCKNELL</t>
-  </si>
-  <si>
-    <t>LAFAYETTE</t>
-  </si>
-  <si>
-    <t>MONTANA TECH</t>
-  </si>
-  <si>
-    <t>PRESBYTERIAN</t>
-  </si>
-  <si>
-    <t>GEORGETOWN-DC</t>
-  </si>
-  <si>
-    <t>DAYTON</t>
-  </si>
-  <si>
-    <t>SOUTH CAROLINA STATE</t>
-  </si>
-  <si>
-    <t>EASTERN WASHINGTON</t>
-  </si>
-  <si>
-    <t>MORNINGSIDE</t>
-  </si>
-  <si>
-    <t>SOUTHERN UTAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT. MARTY S.D. </t>
-  </si>
-  <si>
-    <t>NICHOLLS STATE</t>
-  </si>
-  <si>
-    <t>MONTANA</t>
-  </si>
-  <si>
-    <t>SOUTH DAKOTA</t>
-  </si>
-  <si>
-    <t>ST.XAVIER</t>
-  </si>
-  <si>
-    <t>MAINE</t>
-  </si>
-  <si>
-    <t>SIENA HEIGHTS</t>
-  </si>
-  <si>
-    <t>CAL-SACRAMENTO</t>
-  </si>
-  <si>
-    <t>WAYLAND BAPTIST</t>
-  </si>
-  <si>
-    <t>CENTRAL ARKANSAS</t>
-  </si>
-  <si>
-    <t>MERRIMACK</t>
-  </si>
-  <si>
-    <t>VALPARAISO</t>
-  </si>
-  <si>
-    <t>TEXAS WESLEYAN</t>
-  </si>
-  <si>
-    <t>TENNESSEE STATE</t>
-  </si>
-  <si>
-    <t>CULVER-STOCKTON</t>
-  </si>
-  <si>
-    <t>DICKINSON STATE</t>
-  </si>
-  <si>
-    <t>MONTANA STATE-NORTH</t>
-  </si>
-  <si>
-    <t>McPHERSON</t>
-  </si>
-  <si>
-    <t>MISSOURI BAPTIST</t>
-  </si>
-  <si>
-    <t>DARTMOUTH</t>
-  </si>
-  <si>
-    <t>CUMBERLAND-TN.</t>
-  </si>
-  <si>
-    <t>COLGATE</t>
-  </si>
-  <si>
-    <t>GARDNER-WEBB</t>
-  </si>
-  <si>
-    <t>WILLIAM PENN</t>
-  </si>
-  <si>
-    <t>BRIAR CLIFF</t>
-  </si>
-  <si>
-    <t>AVILA</t>
-  </si>
-  <si>
-    <t>STONEHILL COLLEGE</t>
-  </si>
-  <si>
-    <t>LOUISIANA CHRISTIAN</t>
-  </si>
-  <si>
-    <t>JAMESTOWN</t>
-  </si>
-  <si>
-    <t>ST. ANDREWS- N.C.</t>
-  </si>
-  <si>
-    <t>DELAWARE</t>
-  </si>
-  <si>
-    <t>MADONNA - MICHIGAN</t>
-  </si>
-  <si>
-    <t>ST.THOMAS</t>
-  </si>
-  <si>
-    <t>ST.FRANCIS-ILL</t>
-  </si>
-  <si>
-    <t>ST. THOMAS - FLA</t>
-  </si>
-  <si>
-    <t>DELAWARE STATE</t>
-  </si>
-  <si>
-    <t>ROCKY MOUNTAIN</t>
-  </si>
-  <si>
-    <t>BETHEL KANSAS</t>
-  </si>
-  <si>
-    <t>BRYANT COLLEGE</t>
-  </si>
-  <si>
-    <t>BETHANY KANSAS</t>
-  </si>
-  <si>
-    <t>FLORIDA A&amp;M</t>
-  </si>
-  <si>
-    <t>HASTINGS</t>
-  </si>
-  <si>
-    <t>ARIZONA CHRISTIAN</t>
-  </si>
-  <si>
-    <t>TENNESSEE-MARTIN</t>
-  </si>
-  <si>
-    <t>NORTH DAKOTA STATE</t>
-  </si>
-  <si>
-    <t>POINT</t>
-  </si>
-  <si>
-    <t>MERCER</t>
-  </si>
-  <si>
-    <t>KENNESAW STATE</t>
-  </si>
-  <si>
-    <t>EAST TENNESSEE STATE</t>
-  </si>
-  <si>
-    <t>CAMPBELL</t>
-  </si>
-  <si>
-    <t>GRAMBLING</t>
-  </si>
-  <si>
-    <t>BENEDICTINE-KANSAS</t>
-  </si>
-  <si>
-    <t>SOUTHERN UNIVERSITY</t>
-  </si>
-  <si>
-    <t>TABOR</t>
-  </si>
-  <si>
-    <t>FAULKNER - ALABAMA</t>
-  </si>
-  <si>
-    <t>CAL-DAVIS</t>
-  </si>
-  <si>
-    <t>CORNELL</t>
-  </si>
-  <si>
-    <t>APPRENTICE-NEWPORT NEWS</t>
-  </si>
-  <si>
-    <t>DUQUESNE</t>
-  </si>
-  <si>
-    <t>NEW HAMPSHIRE</t>
-  </si>
-  <si>
-    <t>LINCOLN - CALIFONIA</t>
-  </si>
-  <si>
-    <t>DRAKE</t>
-  </si>
-  <si>
-    <t>JACKSON STATE</t>
-  </si>
-  <si>
-    <t>KEISER - FLA</t>
-  </si>
-  <si>
-    <t>ALABAMA STATE</t>
-  </si>
-  <si>
-    <t>LINSEY WILSON - KY</t>
-  </si>
-  <si>
-    <t>TEXAS SOUTHERN</t>
-  </si>
-  <si>
-    <t>ATLANTIS - FLA</t>
-  </si>
-  <si>
-    <t>OLIVET NAZARENE</t>
-  </si>
-  <si>
-    <t>COLUMBIA</t>
-  </si>
-  <si>
-    <t>ILLINOIS STATE</t>
-  </si>
-  <si>
-    <t>DAKOTA-WESLEYAN SD.</t>
-  </si>
-  <si>
-    <t>EASTERN KENTUCKY</t>
-  </si>
-  <si>
-    <t>CHATTANOOGA-TENNESSEE</t>
-  </si>
-  <si>
-    <t>SO. EAST LOUISIANA</t>
-  </si>
-  <si>
-    <t>UNIV. OF CUMBERLANDS-KY</t>
-  </si>
-  <si>
-    <t>INCARNATE WORD</t>
-  </si>
-  <si>
-    <t>TEXAS COLLEGE</t>
-  </si>
-  <si>
-    <t>SACRED HEART</t>
-  </si>
-  <si>
-    <t>WALDORF</t>
-  </si>
-  <si>
-    <t>MISSOURI VALLEY</t>
-  </si>
-  <si>
-    <t>SOUTH DAKOTA STATE</t>
-  </si>
-  <si>
-    <t>TENNESSEE TECH</t>
-  </si>
-  <si>
-    <t>MAYVILLE STATE</t>
-  </si>
-  <si>
-    <t>VIRGINIA - LYNCHBURG</t>
-  </si>
-  <si>
-    <t>UNION-KY.</t>
-  </si>
-  <si>
-    <t>CONCORDIA-NEBRASKA</t>
-  </si>
-  <si>
-    <t>BAKER</t>
-  </si>
-  <si>
-    <t>CONCORDIA – MICHIGAN</t>
-  </si>
-  <si>
-    <t>RHODE ISLAND</t>
-  </si>
-  <si>
-    <t>CAL-POLY (SAN LOUIS OBISPO)</t>
-  </si>
-  <si>
-    <t>ALBANY-NY</t>
-  </si>
-  <si>
-    <t>IDAHO</t>
-  </si>
-  <si>
-    <t>MURRAY STATE</t>
-  </si>
-  <si>
-    <t>SOUTHERN OREGON</t>
-  </si>
-  <si>
-    <t>DAVIDSON</t>
-  </si>
-  <si>
-    <t>AVE MARIA-FLA</t>
-  </si>
-  <si>
-    <t>ABILENE CHRISTIAN</t>
-  </si>
-  <si>
-    <t>OTTAWA (AZ)</t>
-  </si>
-  <si>
-    <t>PINE BLUFF-ARKANSAS</t>
-  </si>
-  <si>
-    <t>REINHARDT</t>
-  </si>
-  <si>
-    <t>MISSISSIPPI VALLEY STATE</t>
-  </si>
-  <si>
-    <t>ARKANSAS BAPTIST</t>
-  </si>
-  <si>
-    <t>ST.FRANCIS-IND.</t>
-  </si>
-  <si>
-    <t>COLLEGE OF IDAHO</t>
-  </si>
-  <si>
-    <t>GRAND VIEW</t>
-  </si>
-  <si>
-    <t>ROBERT MORRIS - PA</t>
-  </si>
-  <si>
-    <t>SAMFORD</t>
-  </si>
-  <si>
-    <t>MONMOUTH-NJ</t>
-  </si>
-  <si>
-    <t>TAYLOR</t>
-  </si>
-  <si>
-    <t>AUSTIN PEAY</t>
-  </si>
-  <si>
-    <t>TARLETON STATE</t>
-  </si>
-  <si>
-    <t>ALCORN STATE</t>
-  </si>
-  <si>
-    <t>LAMAR</t>
-  </si>
-  <si>
-    <t>STONY BROOK</t>
-  </si>
-  <si>
-    <t>MONTANA - WESTERN</t>
-  </si>
-  <si>
-    <t>MCNEESE STATE</t>
-  </si>
-  <si>
-    <t>EASTERN ILLINOIS</t>
-  </si>
-  <si>
-    <t>SOUTHWESTERN-KANSAS</t>
-  </si>
-  <si>
-    <t>TOWSON</t>
-  </si>
-  <si>
-    <t>SAN DIEGO</t>
-  </si>
-  <si>
-    <t>ST.FRANCIS-PA</t>
-  </si>
-  <si>
-    <t>INDIANA STATE</t>
-  </si>
-  <si>
-    <t>MARIST</t>
-  </si>
-  <si>
-    <t>WEBBER INTERNATIONAL</t>
-  </si>
-  <si>
-    <t>PANHANDLE STATE - OK</t>
-  </si>
-  <si>
-    <t>NORTH DAKOTA</t>
-  </si>
-  <si>
-    <t>PENNSYLVANIA</t>
-  </si>
-  <si>
-    <t>WARNER</t>
-  </si>
-  <si>
-    <t>MIDLAND - NE</t>
-  </si>
-  <si>
-    <t>UTAH TECH</t>
-  </si>
-  <si>
-    <t>KENTUCKY CHRISTIAN</t>
-  </si>
-  <si>
-    <t>HARVARD</t>
-  </si>
-  <si>
-    <t>FLORIDA - MEMORIAL</t>
-  </si>
-  <si>
-    <t>EASTERN OREGON</t>
-  </si>
-  <si>
-    <t>BLUEFIELD - VA</t>
-  </si>
-  <si>
-    <t>BUTLER</t>
-  </si>
-  <si>
-    <t>CARROLL-MONTANA</t>
-  </si>
-  <si>
-    <t>NORTH CAROLINA CENTRAL</t>
-  </si>
-  <si>
-    <t>FORT LAUDERDALE</t>
-  </si>
-  <si>
-    <t>LEHIGH</t>
-  </si>
-  <si>
-    <t>NORTHERN ARIZONA</t>
-  </si>
-  <si>
-    <t>NORTH ALABAMA</t>
-  </si>
-  <si>
-    <t>TAMU - COMMERCE</t>
-  </si>
-  <si>
-    <t>EVANGEL</t>
-  </si>
-  <si>
-    <t>DAKOTA STATE-SD.</t>
-  </si>
-  <si>
-    <t>GRACELAND</t>
-  </si>
-  <si>
-    <t>PORTLAND STATE</t>
-  </si>
-  <si>
-    <t>THE CITADEL</t>
-  </si>
-  <si>
-    <t>LANGSTON</t>
-  </si>
-  <si>
-    <t>STERLING</t>
-  </si>
-  <si>
-    <t>MORGAN STATE</t>
-  </si>
-  <si>
-    <t>FURMAN</t>
-  </si>
-  <si>
-    <t>PIKEVILLE</t>
-  </si>
-  <si>
-    <t>HOWARD</t>
-  </si>
-  <si>
-    <t>HOLY CROSS</t>
+    <t>NO. CAROLINA STATE</t>
+  </si>
+  <si>
+    <t>KENTUCKY</t>
+  </si>
+  <si>
+    <t>BALL STATE</t>
+  </si>
+  <si>
+    <t>LIBERTY</t>
+  </si>
+  <si>
+    <t>CONNECTICUT</t>
+  </si>
+  <si>
+    <t>SOUTHERN CALIFORNIA</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>WESTERN KENTUCKY</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>FLORIDA STATE</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>KANSAS STATE</t>
+  </si>
+  <si>
+    <t>OREGON STATE</t>
+  </si>
+  <si>
+    <t>GEORGIA STATE</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>SOUTH FLORIDA</t>
+  </si>
+  <si>
+    <t>FRESNO STATE</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>SOUTHERN METHODIST</t>
+  </si>
+  <si>
+    <t>UNC - CHARLOTTE</t>
+  </si>
+  <si>
+    <t>CINCINNATI</t>
+  </si>
+  <si>
+    <t>NEVADA-LAS VEGAS</t>
+  </si>
+  <si>
+    <t>PENN STATE</t>
+  </si>
+  <si>
+    <t>AKRON</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>WAKE FOREST</t>
+  </si>
+  <si>
+    <t>NEW MEXICO STATE</t>
+  </si>
+  <si>
+    <t>WASHINGTON STATE</t>
+  </si>
+  <si>
+    <t>BOISE</t>
+  </si>
+  <si>
+    <t>PITTSBURGH</t>
+  </si>
+  <si>
+    <t>SAN DIEGO STATE</t>
+  </si>
+  <si>
+    <t>LOUISVILLE</t>
+  </si>
+  <si>
+    <t>TEXAS-SAN ANTONIO</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>COLORADO STATE</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>SAM HOUSTON</t>
+  </si>
+  <si>
+    <t>HOUSTON</t>
+  </si>
+  <si>
+    <t>MEMPHIS</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI STATE</t>
+  </si>
+  <si>
+    <t>GEORGIA TECH</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>LA - MONROE</t>
+  </si>
+  <si>
+    <t>LOUISIANA STATE</t>
+  </si>
+  <si>
+    <t>BRIGHAM YOUNG</t>
+  </si>
+  <si>
+    <t>JAMES MADISON</t>
+  </si>
+  <si>
+    <t>EASTERN MICHIGAN</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>OKLAHOMA STATE</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>TEXAS CHRISTIAN</t>
+  </si>
+  <si>
+    <t>MIDDLE TENNESSEE STATE</t>
+  </si>
+  <si>
+    <t>KENT STATE</t>
+  </si>
+  <si>
+    <t>WYOMING</t>
+  </si>
+  <si>
+    <t>TEMPLE</t>
+  </si>
+  <si>
+    <t>MIAMI-FL</t>
+  </si>
+  <si>
+    <t>CENTRAL FLORIDA</t>
+  </si>
+  <si>
+    <t>STANFORD</t>
+  </si>
+  <si>
+    <t>SOUTH ALABAMA</t>
+  </si>
+  <si>
+    <t>NOTRE DAME</t>
+  </si>
+  <si>
+    <t>COASTAL CAROLINA</t>
+  </si>
+  <si>
+    <t>SYRACUSE</t>
+  </si>
+  <si>
+    <t>TEXAS-EL PASO</t>
+  </si>
+  <si>
+    <t>ALABAMA</t>
+  </si>
+  <si>
+    <t>AUBURN</t>
+  </si>
+  <si>
+    <t>FLORIDA ATLANTIC</t>
+  </si>
+  <si>
+    <t>BOWLING GREEN</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>NORTHWESTERN</t>
+  </si>
+  <si>
+    <t>TEXAS TECH</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>LOUISIANA TECH</t>
+  </si>
+  <si>
+    <t>MICHIGAN STATE</t>
+  </si>
+  <si>
+    <t>BOSTON COLLEGE</t>
+  </si>
+  <si>
+    <t>BUFFALO</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>PURDUE</t>
+  </si>
+  <si>
+    <t>TEXAS A&amp;M</t>
+  </si>
+  <si>
+    <t>JACKSONVILLE STATE</t>
+  </si>
+  <si>
+    <t>VIRGINIA TECH</t>
+  </si>
+  <si>
+    <t>OLD DOMINION</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>CENTRAL MICHIGAN</t>
+  </si>
+  <si>
+    <t>OHIO UNIV.</t>
+  </si>
+  <si>
+    <t>TROY STATE</t>
+  </si>
+  <si>
+    <t>WISCONSIN</t>
+  </si>
+  <si>
+    <t>EAST CAROLINA</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>IOWA STATE</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>ARKANSAS STATE</t>
+  </si>
+  <si>
+    <t>WESTERN MICHIGAN</t>
+  </si>
+  <si>
+    <t>TOLEDO</t>
+  </si>
+  <si>
+    <t>TULSA</t>
+  </si>
+  <si>
+    <t>GEORGIA SOUTHERN</t>
+  </si>
+  <si>
+    <t>BAYLOR</t>
+  </si>
+  <si>
+    <t>OHIO STATE</t>
+  </si>
+  <si>
+    <t>SOUTHERN MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>ARIZONA STATE</t>
+  </si>
+  <si>
+    <t>MARSHALL</t>
+  </si>
+  <si>
+    <t>APPALACHIAN STATE</t>
+  </si>
+  <si>
+    <t>NORTH TEXAS</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>TULANE</t>
+  </si>
+  <si>
+    <t>FLORIDA INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>TEXAS STATE-SAN MARCOS</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>RUTGERS</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>ALABAMA-BIRMINGHAM</t>
+  </si>
+  <si>
+    <t>NORTHERN ILLINOIS</t>
+  </si>
+  <si>
+    <t>AIR FORCE</t>
+  </si>
+  <si>
+    <t>VANDERBILT</t>
+  </si>
+  <si>
+    <t>UTAH STATE</t>
+  </si>
+  <si>
+    <t>MIAMI OF OHIO</t>
+  </si>
+  <si>
+    <t>CLEMSON</t>
+  </si>
+  <si>
+    <t>SAN JOSE STATE</t>
+  </si>
+  <si>
+    <t>U.C.L.A.</t>
   </si>
 </sst>
 </file>
@@ -2840,7 +2573,7 @@
         <v>463</v>
       </c>
       <c r="E3" t="s">
-        <v>590</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2857,7 +2590,7 @@
         <v>463</v>
       </c>
       <c r="E4" t="s">
-        <v>591</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2874,7 +2607,7 @@
         <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2891,7 +2624,7 @@
         <v>463</v>
       </c>
       <c r="E6" t="s">
-        <v>593</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2908,7 +2641,7 @@
         <v>465</v>
       </c>
       <c r="E7" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2925,7 +2658,7 @@
         <v>463</v>
       </c>
       <c r="E8" t="s">
-        <v>595</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2942,7 +2675,7 @@
         <v>466</v>
       </c>
       <c r="E9" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2959,7 +2692,7 @@
         <v>467</v>
       </c>
       <c r="E10" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2976,7 +2709,7 @@
         <v>463</v>
       </c>
       <c r="E11" t="s">
-        <v>598</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2993,7 +2726,7 @@
         <v>463</v>
       </c>
       <c r="E12" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3010,7 +2743,7 @@
         <v>463</v>
       </c>
       <c r="E13" t="s">
-        <v>600</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3027,7 +2760,7 @@
         <v>468</v>
       </c>
       <c r="E14" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3044,7 +2777,7 @@
         <v>463</v>
       </c>
       <c r="E15" t="s">
-        <v>602</v>
+        <v>463</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3061,7 +2794,7 @@
         <v>469</v>
       </c>
       <c r="E16" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3095,7 +2828,7 @@
         <v>463</v>
       </c>
       <c r="E18" t="s">
-        <v>604</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3112,7 +2845,7 @@
         <v>470</v>
       </c>
       <c r="E19" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3129,7 +2862,7 @@
         <v>463</v>
       </c>
       <c r="E20" t="s">
-        <v>606</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3146,7 +2879,7 @@
         <v>463</v>
       </c>
       <c r="E21" t="s">
-        <v>607</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3163,7 +2896,7 @@
         <v>463</v>
       </c>
       <c r="E22" t="s">
-        <v>608</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3180,7 +2913,7 @@
         <v>471</v>
       </c>
       <c r="E23" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3197,7 +2930,7 @@
         <v>472</v>
       </c>
       <c r="E24" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3214,7 +2947,7 @@
         <v>473</v>
       </c>
       <c r="E25" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3231,7 +2964,7 @@
         <v>463</v>
       </c>
       <c r="E26" t="s">
-        <v>612</v>
+        <v>463</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3248,7 +2981,7 @@
         <v>474</v>
       </c>
       <c r="E27" t="s">
-        <v>613</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3265,7 +2998,7 @@
         <v>475</v>
       </c>
       <c r="E28" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3282,7 +3015,7 @@
         <v>463</v>
       </c>
       <c r="E29" t="s">
-        <v>615</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3299,7 +3032,7 @@
         <v>463</v>
       </c>
       <c r="E30" t="s">
-        <v>616</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3316,7 +3049,7 @@
         <v>476</v>
       </c>
       <c r="E31" t="s">
-        <v>617</v>
+        <v>602</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3333,7 +3066,7 @@
         <v>463</v>
       </c>
       <c r="E32" t="s">
-        <v>618</v>
+        <v>463</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3350,7 +3083,7 @@
         <v>477</v>
       </c>
       <c r="E33" t="s">
-        <v>619</v>
+        <v>603</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3364,10 +3097,10 @@
         <v>266</v>
       </c>
       <c r="D34" t="s">
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="E34" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3381,10 +3114,10 @@
         <v>267</v>
       </c>
       <c r="D35" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E35" t="s">
-        <v>621</v>
+        <v>605</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3398,10 +3131,10 @@
         <v>268</v>
       </c>
       <c r="D36" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E36" t="s">
-        <v>622</v>
+        <v>606</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3418,7 +3151,7 @@
         <v>463</v>
       </c>
       <c r="E37" t="s">
-        <v>623</v>
+        <v>463</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3452,7 +3185,7 @@
         <v>463</v>
       </c>
       <c r="E39" t="s">
-        <v>624</v>
+        <v>463</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3466,10 +3199,10 @@
         <v>272</v>
       </c>
       <c r="D40" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E40" t="s">
-        <v>625</v>
+        <v>607</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3486,7 +3219,7 @@
         <v>463</v>
       </c>
       <c r="E41" t="s">
-        <v>626</v>
+        <v>463</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3503,7 +3236,7 @@
         <v>463</v>
       </c>
       <c r="E42" t="s">
-        <v>627</v>
+        <v>463</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3520,7 +3253,7 @@
         <v>463</v>
       </c>
       <c r="E43" t="s">
-        <v>628</v>
+        <v>463</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3537,7 +3270,7 @@
         <v>463</v>
       </c>
       <c r="E44" t="s">
-        <v>629</v>
+        <v>463</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3551,10 +3284,10 @@
         <v>277</v>
       </c>
       <c r="D45" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E45" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3571,7 +3304,7 @@
         <v>463</v>
       </c>
       <c r="E46" t="s">
-        <v>631</v>
+        <v>463</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3602,10 +3335,10 @@
         <v>280</v>
       </c>
       <c r="D48" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="E48" t="s">
-        <v>632</v>
+        <v>463</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3622,7 +3355,7 @@
         <v>463</v>
       </c>
       <c r="E49" t="s">
-        <v>633</v>
+        <v>609</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3639,7 +3372,7 @@
         <v>483</v>
       </c>
       <c r="E50" t="s">
-        <v>634</v>
+        <v>610</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3656,7 +3389,7 @@
         <v>484</v>
       </c>
       <c r="E51" t="s">
-        <v>635</v>
+        <v>611</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3673,7 +3406,7 @@
         <v>463</v>
       </c>
       <c r="E52" t="s">
-        <v>636</v>
+        <v>612</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3690,7 +3423,7 @@
         <v>485</v>
       </c>
       <c r="E53" t="s">
-        <v>637</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3707,7 +3440,7 @@
         <v>486</v>
       </c>
       <c r="E54" t="s">
-        <v>638</v>
+        <v>614</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3724,7 +3457,7 @@
         <v>487</v>
       </c>
       <c r="E55" t="s">
-        <v>639</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3741,7 +3474,7 @@
         <v>463</v>
       </c>
       <c r="E56" t="s">
-        <v>640</v>
+        <v>463</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3758,7 +3491,7 @@
         <v>488</v>
       </c>
       <c r="E57" t="s">
-        <v>641</v>
+        <v>463</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3775,7 +3508,7 @@
         <v>489</v>
       </c>
       <c r="E58" t="s">
-        <v>642</v>
+        <v>615</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3792,7 +3525,7 @@
         <v>490</v>
       </c>
       <c r="E59" t="s">
-        <v>643</v>
+        <v>616</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3806,10 +3539,10 @@
         <v>292</v>
       </c>
       <c r="D60" t="s">
-        <v>463</v>
+        <v>491</v>
       </c>
       <c r="E60" t="s">
-        <v>644</v>
+        <v>463</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3823,10 +3556,10 @@
         <v>293</v>
       </c>
       <c r="D61" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E61" t="s">
-        <v>645</v>
+        <v>617</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3840,10 +3573,10 @@
         <v>294</v>
       </c>
       <c r="D62" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E62" t="s">
-        <v>646</v>
+        <v>618</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3857,10 +3590,10 @@
         <v>295</v>
       </c>
       <c r="D63" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E63" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3874,10 +3607,10 @@
         <v>296</v>
       </c>
       <c r="D64" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E64" t="s">
-        <v>648</v>
+        <v>620</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3894,7 +3627,7 @@
         <v>463</v>
       </c>
       <c r="E65" t="s">
-        <v>649</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3908,10 +3641,10 @@
         <v>298</v>
       </c>
       <c r="D66" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E66" t="s">
-        <v>650</v>
+        <v>621</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3928,7 +3661,7 @@
         <v>463</v>
       </c>
       <c r="E67" t="s">
-        <v>651</v>
+        <v>463</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3942,10 +3675,10 @@
         <v>300</v>
       </c>
       <c r="D68" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E68" t="s">
-        <v>652</v>
+        <v>463</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3962,7 +3695,7 @@
         <v>463</v>
       </c>
       <c r="E69" t="s">
-        <v>653</v>
+        <v>622</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3976,10 +3709,10 @@
         <v>302</v>
       </c>
       <c r="D70" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E70" t="s">
-        <v>654</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3996,7 +3729,7 @@
         <v>463</v>
       </c>
       <c r="E71" t="s">
-        <v>655</v>
+        <v>623</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4013,7 +3746,7 @@
         <v>463</v>
       </c>
       <c r="E72" t="s">
-        <v>656</v>
+        <v>624</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -4027,10 +3760,10 @@
         <v>305</v>
       </c>
       <c r="D73" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E73" t="s">
-        <v>657</v>
+        <v>625</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -4044,10 +3777,10 @@
         <v>306</v>
       </c>
       <c r="D74" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E74" t="s">
-        <v>658</v>
+        <v>626</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4064,7 +3797,7 @@
         <v>463</v>
       </c>
       <c r="E75" t="s">
-        <v>659</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -4078,10 +3811,10 @@
         <v>308</v>
       </c>
       <c r="D76" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E76" t="s">
-        <v>660</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4098,7 +3831,7 @@
         <v>463</v>
       </c>
       <c r="E77" t="s">
-        <v>661</v>
+        <v>627</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4115,7 +3848,7 @@
         <v>463</v>
       </c>
       <c r="E78" t="s">
-        <v>662</v>
+        <v>463</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4129,10 +3862,10 @@
         <v>311</v>
       </c>
       <c r="D79" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E79" t="s">
-        <v>663</v>
+        <v>628</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -4149,7 +3882,7 @@
         <v>463</v>
       </c>
       <c r="E80" t="s">
-        <v>664</v>
+        <v>463</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -4163,10 +3896,10 @@
         <v>313</v>
       </c>
       <c r="D81" t="s">
-        <v>502</v>
+        <v>463</v>
       </c>
       <c r="E81" t="s">
-        <v>665</v>
+        <v>463</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -4183,7 +3916,7 @@
         <v>503</v>
       </c>
       <c r="E82" t="s">
-        <v>666</v>
+        <v>629</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -4200,7 +3933,7 @@
         <v>504</v>
       </c>
       <c r="E83" t="s">
-        <v>667</v>
+        <v>630</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -4217,7 +3950,7 @@
         <v>463</v>
       </c>
       <c r="E84" t="s">
-        <v>668</v>
+        <v>463</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -4268,7 +4001,7 @@
         <v>463</v>
       </c>
       <c r="E87" t="s">
-        <v>669</v>
+        <v>463</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -4285,7 +4018,7 @@
         <v>463</v>
       </c>
       <c r="E88" t="s">
-        <v>670</v>
+        <v>463</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4302,7 +4035,7 @@
         <v>463</v>
       </c>
       <c r="E89" t="s">
-        <v>671</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4319,7 +4052,7 @@
         <v>463</v>
       </c>
       <c r="E90" t="s">
-        <v>672</v>
+        <v>463</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4336,7 +4069,7 @@
         <v>505</v>
       </c>
       <c r="E91" t="s">
-        <v>673</v>
+        <v>631</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4353,7 +4086,7 @@
         <v>506</v>
       </c>
       <c r="E92" t="s">
-        <v>674</v>
+        <v>632</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4370,7 +4103,7 @@
         <v>507</v>
       </c>
       <c r="E93" t="s">
-        <v>675</v>
+        <v>633</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -4384,10 +4117,10 @@
         <v>326</v>
       </c>
       <c r="D94" t="s">
-        <v>463</v>
+        <v>508</v>
       </c>
       <c r="E94" t="s">
-        <v>676</v>
+        <v>634</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4401,10 +4134,10 @@
         <v>327</v>
       </c>
       <c r="D95" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E95" t="s">
-        <v>677</v>
+        <v>635</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4418,10 +4151,10 @@
         <v>328</v>
       </c>
       <c r="D96" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E96" t="s">
-        <v>678</v>
+        <v>636</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4435,10 +4168,10 @@
         <v>329</v>
       </c>
       <c r="D97" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="E97" t="s">
-        <v>679</v>
+        <v>463</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4455,7 +4188,7 @@
         <v>511</v>
       </c>
       <c r="E98" t="s">
-        <v>680</v>
+        <v>637</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4472,7 +4205,7 @@
         <v>512</v>
       </c>
       <c r="E99" t="s">
-        <v>681</v>
+        <v>638</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4489,7 +4222,7 @@
         <v>463</v>
       </c>
       <c r="E100" t="s">
-        <v>682</v>
+        <v>463</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4506,7 +4239,7 @@
         <v>513</v>
       </c>
       <c r="E101" t="s">
-        <v>683</v>
+        <v>639</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4523,7 +4256,7 @@
         <v>463</v>
       </c>
       <c r="E102" t="s">
-        <v>684</v>
+        <v>463</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4557,7 +4290,7 @@
         <v>463</v>
       </c>
       <c r="E104" t="s">
-        <v>685</v>
+        <v>463</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4574,7 +4307,7 @@
         <v>514</v>
       </c>
       <c r="E105" t="s">
-        <v>686</v>
+        <v>640</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4591,7 +4324,7 @@
         <v>515</v>
       </c>
       <c r="E106" t="s">
-        <v>687</v>
+        <v>463</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4625,7 +4358,7 @@
         <v>516</v>
       </c>
       <c r="E108" t="s">
-        <v>688</v>
+        <v>641</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4642,7 +4375,7 @@
         <v>517</v>
       </c>
       <c r="E109" t="s">
-        <v>689</v>
+        <v>642</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4659,7 +4392,7 @@
         <v>518</v>
       </c>
       <c r="E110" t="s">
-        <v>690</v>
+        <v>643</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4676,7 +4409,7 @@
         <v>519</v>
       </c>
       <c r="E111" t="s">
-        <v>691</v>
+        <v>644</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4693,7 +4426,7 @@
         <v>520</v>
       </c>
       <c r="E112" t="s">
-        <v>692</v>
+        <v>645</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4710,7 +4443,7 @@
         <v>521</v>
       </c>
       <c r="E113" t="s">
-        <v>693</v>
+        <v>646</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4727,7 +4460,7 @@
         <v>522</v>
       </c>
       <c r="E114" t="s">
-        <v>694</v>
+        <v>647</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4744,7 +4477,7 @@
         <v>463</v>
       </c>
       <c r="E115" t="s">
-        <v>695</v>
+        <v>463</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4761,7 +4494,7 @@
         <v>463</v>
       </c>
       <c r="E116" t="s">
-        <v>696</v>
+        <v>463</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4778,7 +4511,7 @@
         <v>463</v>
       </c>
       <c r="E117" t="s">
-        <v>697</v>
+        <v>463</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4795,7 +4528,7 @@
         <v>523</v>
       </c>
       <c r="E118" t="s">
-        <v>698</v>
+        <v>648</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4812,7 +4545,7 @@
         <v>524</v>
       </c>
       <c r="E119" t="s">
-        <v>699</v>
+        <v>649</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4829,7 +4562,7 @@
         <v>463</v>
       </c>
       <c r="E120" t="s">
-        <v>700</v>
+        <v>650</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4846,7 +4579,7 @@
         <v>463</v>
       </c>
       <c r="E121" t="s">
-        <v>701</v>
+        <v>463</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4863,7 +4596,7 @@
         <v>525</v>
       </c>
       <c r="E122" t="s">
-        <v>702</v>
+        <v>651</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4877,10 +4610,10 @@
         <v>355</v>
       </c>
       <c r="D123" t="s">
-        <v>463</v>
+        <v>526</v>
       </c>
       <c r="E123" t="s">
-        <v>703</v>
+        <v>652</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4897,7 +4630,7 @@
         <v>463</v>
       </c>
       <c r="E124" t="s">
-        <v>704</v>
+        <v>463</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4914,7 +4647,7 @@
         <v>463</v>
       </c>
       <c r="E125" t="s">
-        <v>705</v>
+        <v>463</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4928,10 +4661,10 @@
         <v>358</v>
       </c>
       <c r="D126" t="s">
-        <v>463</v>
+        <v>527</v>
       </c>
       <c r="E126" t="s">
-        <v>706</v>
+        <v>463</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4948,7 +4681,7 @@
         <v>463</v>
       </c>
       <c r="E127" t="s">
-        <v>707</v>
+        <v>463</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -4962,10 +4695,10 @@
         <v>360</v>
       </c>
       <c r="D128" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E128" t="s">
-        <v>708</v>
+        <v>653</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4979,10 +4712,10 @@
         <v>361</v>
       </c>
       <c r="D129" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E129" t="s">
-        <v>709</v>
+        <v>654</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4996,10 +4729,10 @@
         <v>362</v>
       </c>
       <c r="D130" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E130" t="s">
-        <v>710</v>
+        <v>655</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -5013,10 +4746,10 @@
         <v>363</v>
       </c>
       <c r="D131" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E131" t="s">
-        <v>711</v>
+        <v>656</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -5033,7 +4766,7 @@
         <v>463</v>
       </c>
       <c r="E132" t="s">
-        <v>712</v>
+        <v>463</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -5047,10 +4780,10 @@
         <v>365</v>
       </c>
       <c r="D133" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="E133" t="s">
-        <v>713</v>
+        <v>657</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -5067,7 +4800,7 @@
         <v>463</v>
       </c>
       <c r="E134" t="s">
-        <v>714</v>
+        <v>463</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -5081,10 +4814,10 @@
         <v>367</v>
       </c>
       <c r="D135" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E135" t="s">
-        <v>715</v>
+        <v>658</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -5098,10 +4831,10 @@
         <v>368</v>
       </c>
       <c r="D136" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E136" t="s">
-        <v>716</v>
+        <v>659</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -5115,10 +4848,10 @@
         <v>369</v>
       </c>
       <c r="D137" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E137" t="s">
-        <v>717</v>
+        <v>660</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -5132,10 +4865,10 @@
         <v>370</v>
       </c>
       <c r="D138" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E138" t="s">
-        <v>718</v>
+        <v>661</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -5149,10 +4882,10 @@
         <v>371</v>
       </c>
       <c r="D139" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E139" t="s">
-        <v>719</v>
+        <v>662</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -5166,10 +4899,10 @@
         <v>372</v>
       </c>
       <c r="D140" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E140" t="s">
-        <v>720</v>
+        <v>663</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -5183,10 +4916,10 @@
         <v>373</v>
       </c>
       <c r="D141" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E141" t="s">
-        <v>721</v>
+        <v>664</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -5200,10 +4933,10 @@
         <v>374</v>
       </c>
       <c r="D142" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E142" t="s">
-        <v>722</v>
+        <v>665</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -5220,7 +4953,7 @@
         <v>463</v>
       </c>
       <c r="E143" t="s">
-        <v>723</v>
+        <v>666</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -5237,7 +4970,7 @@
         <v>463</v>
       </c>
       <c r="E144" t="s">
-        <v>724</v>
+        <v>463</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -5251,10 +4984,10 @@
         <v>377</v>
       </c>
       <c r="D145" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E145" t="s">
-        <v>725</v>
+        <v>667</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -5268,10 +5001,10 @@
         <v>378</v>
       </c>
       <c r="D146" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E146" t="s">
-        <v>726</v>
+        <v>668</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -5285,10 +5018,10 @@
         <v>379</v>
       </c>
       <c r="D147" t="s">
-        <v>541</v>
+        <v>463</v>
       </c>
       <c r="E147" t="s">
-        <v>727</v>
+        <v>463</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -5302,10 +5035,10 @@
         <v>380</v>
       </c>
       <c r="D148" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E148" t="s">
-        <v>728</v>
+        <v>669</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5319,10 +5052,10 @@
         <v>381</v>
       </c>
       <c r="D149" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E149" t="s">
-        <v>729</v>
+        <v>670</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5336,10 +5069,10 @@
         <v>382</v>
       </c>
       <c r="D150" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E150" t="s">
-        <v>730</v>
+        <v>671</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5353,10 +5086,10 @@
         <v>383</v>
       </c>
       <c r="D151" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E151" t="s">
-        <v>731</v>
+        <v>672</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5370,10 +5103,10 @@
         <v>384</v>
       </c>
       <c r="D152" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E152" t="s">
-        <v>732</v>
+        <v>673</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5387,10 +5120,10 @@
         <v>385</v>
       </c>
       <c r="D153" t="s">
-        <v>547</v>
+        <v>463</v>
       </c>
       <c r="E153" t="s">
-        <v>733</v>
+        <v>674</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5407,7 +5140,7 @@
         <v>548</v>
       </c>
       <c r="E154" t="s">
-        <v>734</v>
+        <v>675</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5424,7 +5157,7 @@
         <v>549</v>
       </c>
       <c r="E155" t="s">
-        <v>735</v>
+        <v>676</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5441,7 +5174,7 @@
         <v>463</v>
       </c>
       <c r="E156" t="s">
-        <v>736</v>
+        <v>463</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5475,7 +5208,7 @@
         <v>550</v>
       </c>
       <c r="E158" t="s">
-        <v>737</v>
+        <v>677</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5492,7 +5225,7 @@
         <v>463</v>
       </c>
       <c r="E159" t="s">
-        <v>738</v>
+        <v>463</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5506,10 +5239,10 @@
         <v>392</v>
       </c>
       <c r="D160" t="s">
-        <v>463</v>
+        <v>551</v>
       </c>
       <c r="E160" t="s">
-        <v>739</v>
+        <v>463</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -5523,10 +5256,10 @@
         <v>393</v>
       </c>
       <c r="D161" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E161" t="s">
-        <v>740</v>
+        <v>463</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -5540,10 +5273,10 @@
         <v>394</v>
       </c>
       <c r="D162" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E162" t="s">
-        <v>741</v>
+        <v>678</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5560,7 +5293,7 @@
         <v>463</v>
       </c>
       <c r="E163" t="s">
-        <v>742</v>
+        <v>679</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5577,7 +5310,7 @@
         <v>463</v>
       </c>
       <c r="E164" t="s">
-        <v>396</v>
+        <v>463</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5594,7 +5327,7 @@
         <v>463</v>
       </c>
       <c r="E165" t="s">
-        <v>743</v>
+        <v>463</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5608,10 +5341,10 @@
         <v>398</v>
       </c>
       <c r="D166" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E166" t="s">
-        <v>744</v>
+        <v>680</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5625,10 +5358,10 @@
         <v>399</v>
       </c>
       <c r="D167" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E167" t="s">
-        <v>745</v>
+        <v>681</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5642,10 +5375,10 @@
         <v>400</v>
       </c>
       <c r="D168" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E168" t="s">
-        <v>746</v>
+        <v>682</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5676,10 +5409,10 @@
         <v>402</v>
       </c>
       <c r="D170" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E170" t="s">
-        <v>747</v>
+        <v>683</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5693,10 +5426,10 @@
         <v>403</v>
       </c>
       <c r="D171" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E171" t="s">
-        <v>748</v>
+        <v>684</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5710,10 +5443,10 @@
         <v>404</v>
       </c>
       <c r="D172" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E172" t="s">
-        <v>749</v>
+        <v>685</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5727,10 +5460,10 @@
         <v>405</v>
       </c>
       <c r="D173" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E173" t="s">
-        <v>750</v>
+        <v>686</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5744,10 +5477,10 @@
         <v>406</v>
       </c>
       <c r="D174" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E174" t="s">
-        <v>751</v>
+        <v>687</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5761,10 +5494,10 @@
         <v>407</v>
       </c>
       <c r="D175" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E175" t="s">
-        <v>752</v>
+        <v>688</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5778,10 +5511,10 @@
         <v>408</v>
       </c>
       <c r="D176" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E176" t="s">
-        <v>753</v>
+        <v>689</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5798,7 +5531,7 @@
         <v>463</v>
       </c>
       <c r="E177" t="s">
-        <v>754</v>
+        <v>463</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -5815,7 +5548,7 @@
         <v>463</v>
       </c>
       <c r="E178" t="s">
-        <v>755</v>
+        <v>463</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -5829,10 +5562,10 @@
         <v>411</v>
       </c>
       <c r="D179" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E179" t="s">
-        <v>756</v>
+        <v>690</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5846,10 +5579,10 @@
         <v>412</v>
       </c>
       <c r="D180" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E180" t="s">
-        <v>757</v>
+        <v>691</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5863,10 +5596,10 @@
         <v>413</v>
       </c>
       <c r="D181" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E181" t="s">
-        <v>758</v>
+        <v>692</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5883,7 +5616,7 @@
         <v>463</v>
       </c>
       <c r="E182" t="s">
-        <v>759</v>
+        <v>463</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5917,7 +5650,7 @@
         <v>463</v>
       </c>
       <c r="E184" t="s">
-        <v>760</v>
+        <v>463</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -5934,7 +5667,7 @@
         <v>463</v>
       </c>
       <c r="E185" t="s">
-        <v>761</v>
+        <v>463</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -5951,7 +5684,7 @@
         <v>463</v>
       </c>
       <c r="E186" t="s">
-        <v>762</v>
+        <v>463</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -5965,10 +5698,10 @@
         <v>419</v>
       </c>
       <c r="D187" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E187" t="s">
-        <v>763</v>
+        <v>463</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5985,7 +5718,7 @@
         <v>463</v>
       </c>
       <c r="E188" t="s">
-        <v>764</v>
+        <v>463</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5999,10 +5732,10 @@
         <v>421</v>
       </c>
       <c r="D189" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E189" t="s">
-        <v>765</v>
+        <v>693</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -6019,7 +5752,7 @@
         <v>463</v>
       </c>
       <c r="E190" t="s">
-        <v>766</v>
+        <v>463</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -6033,10 +5766,10 @@
         <v>423</v>
       </c>
       <c r="D191" t="s">
-        <v>463</v>
+        <v>569</v>
       </c>
       <c r="E191" t="s">
-        <v>767</v>
+        <v>694</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -6050,10 +5783,10 @@
         <v>424</v>
       </c>
       <c r="D192" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E192" t="s">
-        <v>768</v>
+        <v>695</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -6070,7 +5803,7 @@
         <v>463</v>
       </c>
       <c r="E193" t="s">
-        <v>769</v>
+        <v>463</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -6084,10 +5817,10 @@
         <v>426</v>
       </c>
       <c r="D194" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="E194" t="s">
-        <v>770</v>
+        <v>426</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -6101,10 +5834,10 @@
         <v>427</v>
       </c>
       <c r="D195" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="E195" t="s">
-        <v>771</v>
+        <v>696</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -6118,10 +5851,10 @@
         <v>428</v>
       </c>
       <c r="D196" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E196" t="s">
-        <v>772</v>
+        <v>697</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -6138,7 +5871,7 @@
         <v>463</v>
       </c>
       <c r="E197" t="s">
-        <v>773</v>
+        <v>463</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -6172,7 +5905,7 @@
         <v>463</v>
       </c>
       <c r="E199" t="s">
-        <v>774</v>
+        <v>698</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -6186,10 +5919,10 @@
         <v>432</v>
       </c>
       <c r="D200" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="E200" t="s">
-        <v>775</v>
+        <v>699</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -6203,10 +5936,10 @@
         <v>433</v>
       </c>
       <c r="D201" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E201" t="s">
-        <v>776</v>
+        <v>700</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -6223,7 +5956,7 @@
         <v>463</v>
       </c>
       <c r="E202" t="s">
-        <v>777</v>
+        <v>463</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -6237,10 +5970,10 @@
         <v>435</v>
       </c>
       <c r="D203" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E203" t="s">
-        <v>778</v>
+        <v>701</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -6254,10 +5987,10 @@
         <v>436</v>
       </c>
       <c r="D204" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="E204" t="s">
-        <v>779</v>
+        <v>436</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -6274,7 +6007,7 @@
         <v>463</v>
       </c>
       <c r="E205" t="s">
-        <v>780</v>
+        <v>463</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -6291,7 +6024,7 @@
         <v>463</v>
       </c>
       <c r="E206" t="s">
-        <v>781</v>
+        <v>463</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -6305,10 +6038,10 @@
         <v>439</v>
       </c>
       <c r="D207" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E207" t="s">
-        <v>782</v>
+        <v>702</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -6322,10 +6055,10 @@
         <v>440</v>
       </c>
       <c r="D208" t="s">
-        <v>577</v>
+        <v>463</v>
       </c>
       <c r="E208" t="s">
-        <v>783</v>
+        <v>703</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6339,10 +6072,10 @@
         <v>441</v>
       </c>
       <c r="D209" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E209" t="s">
-        <v>784</v>
+        <v>704</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6356,10 +6089,10 @@
         <v>442</v>
       </c>
       <c r="D210" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E210" t="s">
-        <v>785</v>
+        <v>705</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6376,7 +6109,7 @@
         <v>463</v>
       </c>
       <c r="E211" t="s">
-        <v>786</v>
+        <v>463</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -6390,10 +6123,10 @@
         <v>444</v>
       </c>
       <c r="D212" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E212" t="s">
-        <v>787</v>
+        <v>706</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6410,7 +6143,7 @@
         <v>463</v>
       </c>
       <c r="E213" t="s">
-        <v>788</v>
+        <v>463</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6427,7 +6160,7 @@
         <v>463</v>
       </c>
       <c r="E214" t="s">
-        <v>789</v>
+        <v>707</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6441,10 +6174,10 @@
         <v>447</v>
       </c>
       <c r="D215" t="s">
-        <v>581</v>
+        <v>463</v>
       </c>
       <c r="E215" t="s">
-        <v>790</v>
+        <v>708</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6461,7 +6194,7 @@
         <v>463</v>
       </c>
       <c r="E216" t="s">
-        <v>791</v>
+        <v>463</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6478,7 +6211,7 @@
         <v>582</v>
       </c>
       <c r="E217" t="s">
-        <v>792</v>
+        <v>709</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6495,7 +6228,7 @@
         <v>583</v>
       </c>
       <c r="E218" t="s">
-        <v>793</v>
+        <v>710</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6512,7 +6245,7 @@
         <v>463</v>
       </c>
       <c r="E219" t="s">
-        <v>794</v>
+        <v>463</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -6529,7 +6262,7 @@
         <v>463</v>
       </c>
       <c r="E220" t="s">
-        <v>795</v>
+        <v>463</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -6546,7 +6279,7 @@
         <v>584</v>
       </c>
       <c r="E221" t="s">
-        <v>796</v>
+        <v>711</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6580,7 +6313,7 @@
         <v>585</v>
       </c>
       <c r="E223" t="s">
-        <v>797</v>
+        <v>712</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -6597,7 +6330,7 @@
         <v>586</v>
       </c>
       <c r="E224" t="s">
-        <v>798</v>
+        <v>713</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6614,7 +6347,7 @@
         <v>463</v>
       </c>
       <c r="E225" t="s">
-        <v>799</v>
+        <v>463</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -6631,7 +6364,7 @@
         <v>587</v>
       </c>
       <c r="E226" t="s">
-        <v>800</v>
+        <v>714</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6648,7 +6381,7 @@
         <v>463</v>
       </c>
       <c r="E227" t="s">
-        <v>801</v>
+        <v>463</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -6665,7 +6398,7 @@
         <v>463</v>
       </c>
       <c r="E228" t="s">
-        <v>802</v>
+        <v>715</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6682,7 +6415,7 @@
         <v>588</v>
       </c>
       <c r="E229" t="s">
-        <v>803</v>
+        <v>461</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -6699,7 +6432,7 @@
         <v>463</v>
       </c>
       <c r="E230" t="s">
-        <v>804</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge spreadsheet works, except overrides
</commit_message>
<xml_diff>
--- a/data/merge.xlsx
+++ b/data/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="717">
   <si>
     <t>Index</t>
   </si>
@@ -1411,154 +1411,160 @@
     <t>Kentucky</t>
   </si>
   <si>
+    <t>NC State</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>W Virginia</t>
+  </si>
+  <si>
+    <t>W Kentucky</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Florida St</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Kansas St</t>
+  </si>
+  <si>
+    <t>U Mass</t>
+  </si>
+  <si>
+    <t>Oregon St</t>
+  </si>
+  <si>
+    <t>Georgia St</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>S Florida</t>
+  </si>
+  <si>
+    <t>Fresno St</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>N Carolina</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>Penn St</t>
+  </si>
+  <si>
+    <t>Akron</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>VA Tech</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Wake Forest</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>N Mex State</t>
+  </si>
+  <si>
+    <t>Wash State</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>San Diego St</t>
+  </si>
+  <si>
+    <t>App State</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Colorado St</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Miss State</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TX Christian</t>
+  </si>
+  <si>
+    <t>GA Tech</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>UL Monroe</t>
+  </si>
+  <si>
+    <t>LA Tech</t>
+  </si>
+  <si>
+    <t>S Methodist</t>
+  </si>
+  <si>
+    <t>James Mad</t>
+  </si>
+  <si>
+    <t>E Michigan</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Oklahoma St</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
     <t>Ball St</t>
-  </si>
-  <si>
-    <t>Liberty</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>W Virginia</t>
-  </si>
-  <si>
-    <t>W Kentucky</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Florida St</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Kansas St</t>
-  </si>
-  <si>
-    <t>U Mass</t>
-  </si>
-  <si>
-    <t>Oregon St</t>
-  </si>
-  <si>
-    <t>Georgia St</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>S Florida</t>
-  </si>
-  <si>
-    <t>Fresno St</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>N Carolina</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Cincinnati</t>
-  </si>
-  <si>
-    <t>Penn St</t>
-  </si>
-  <si>
-    <t>Akron</t>
-  </si>
-  <si>
-    <t>Duke</t>
-  </si>
-  <si>
-    <t>VA Tech</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Wake Forest</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>N Mex State</t>
-  </si>
-  <si>
-    <t>Wash State</t>
-  </si>
-  <si>
-    <t>Louisville</t>
-  </si>
-  <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
-    <t>San Diego St</t>
-  </si>
-  <si>
-    <t>App State</t>
-  </si>
-  <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Colorado St</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Army</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Miss State</t>
-  </si>
-  <si>
-    <t>GA Tech</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>UL Monroe</t>
-  </si>
-  <si>
-    <t>LA Tech</t>
-  </si>
-  <si>
-    <t>S Methodist</t>
-  </si>
-  <si>
-    <t>James Mad</t>
-  </si>
-  <si>
-    <t>E Michigan</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Oklahoma St</t>
-  </si>
-  <si>
-    <t>Kansas</t>
   </si>
   <si>
     <t>Arkansas</t>
@@ -2553,7 +2559,7 @@
         <v>463</v>
       </c>
       <c r="E2" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2604,7 +2610,7 @@
         <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2638,7 +2644,7 @@
         <v>465</v>
       </c>
       <c r="E7" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2672,7 +2678,7 @@
         <v>466</v>
       </c>
       <c r="E9" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2689,7 +2695,7 @@
         <v>467</v>
       </c>
       <c r="E10" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2723,7 +2729,7 @@
         <v>463</v>
       </c>
       <c r="E12" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2757,7 +2763,7 @@
         <v>468</v>
       </c>
       <c r="E14" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2791,7 +2797,7 @@
         <v>469</v>
       </c>
       <c r="E16" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2842,7 +2848,7 @@
         <v>470</v>
       </c>
       <c r="E19" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2910,7 +2916,7 @@
         <v>471</v>
       </c>
       <c r="E23" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2927,7 +2933,7 @@
         <v>472</v>
       </c>
       <c r="E24" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2944,7 +2950,7 @@
         <v>473</v>
       </c>
       <c r="E25" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2995,7 +3001,7 @@
         <v>475</v>
       </c>
       <c r="E28" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3046,7 +3052,7 @@
         <v>476</v>
       </c>
       <c r="E31" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3080,7 +3086,7 @@
         <v>477</v>
       </c>
       <c r="E33" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3097,7 +3103,7 @@
         <v>478</v>
       </c>
       <c r="E34" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3114,7 +3120,7 @@
         <v>479</v>
       </c>
       <c r="E35" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3131,7 +3137,7 @@
         <v>480</v>
       </c>
       <c r="E36" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3199,7 +3205,7 @@
         <v>481</v>
       </c>
       <c r="E40" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3284,7 +3290,7 @@
         <v>482</v>
       </c>
       <c r="E45" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3352,7 +3358,7 @@
         <v>463</v>
       </c>
       <c r="E49" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3369,7 +3375,7 @@
         <v>483</v>
       </c>
       <c r="E50" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3386,7 +3392,7 @@
         <v>484</v>
       </c>
       <c r="E51" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3403,7 +3409,7 @@
         <v>463</v>
       </c>
       <c r="E52" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3420,7 +3426,7 @@
         <v>485</v>
       </c>
       <c r="E53" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3437,7 +3443,7 @@
         <v>486</v>
       </c>
       <c r="E54" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3505,7 +3511,7 @@
         <v>489</v>
       </c>
       <c r="E58" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3522,7 +3528,7 @@
         <v>490</v>
       </c>
       <c r="E59" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3556,7 +3562,7 @@
         <v>492</v>
       </c>
       <c r="E61" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3573,7 +3579,7 @@
         <v>493</v>
       </c>
       <c r="E62" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3590,7 +3596,7 @@
         <v>494</v>
       </c>
       <c r="E63" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3607,7 +3613,7 @@
         <v>495</v>
       </c>
       <c r="E64" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3641,7 +3647,7 @@
         <v>496</v>
       </c>
       <c r="E66" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3692,7 +3698,7 @@
         <v>463</v>
       </c>
       <c r="E69" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3726,7 +3732,7 @@
         <v>463</v>
       </c>
       <c r="E71" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3743,7 +3749,7 @@
         <v>463</v>
       </c>
       <c r="E72" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3760,7 +3766,7 @@
         <v>499</v>
       </c>
       <c r="E73" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3777,7 +3783,7 @@
         <v>500</v>
       </c>
       <c r="E74" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3828,7 +3834,7 @@
         <v>463</v>
       </c>
       <c r="E77" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3862,7 +3868,7 @@
         <v>502</v>
       </c>
       <c r="E79" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3913,7 +3919,7 @@
         <v>503</v>
       </c>
       <c r="E82" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3930,7 +3936,7 @@
         <v>504</v>
       </c>
       <c r="E83" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3961,7 +3967,7 @@
         <v>317</v>
       </c>
       <c r="D85" t="s">
-        <v>463</v>
+        <v>505</v>
       </c>
       <c r="E85" t="s">
         <v>463</v>
@@ -4063,10 +4069,10 @@
         <v>323</v>
       </c>
       <c r="D91" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E91" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4080,10 +4086,10 @@
         <v>324</v>
       </c>
       <c r="D92" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E92" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4097,10 +4103,10 @@
         <v>325</v>
       </c>
       <c r="D93" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E93" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -4114,10 +4120,10 @@
         <v>326</v>
       </c>
       <c r="D94" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E94" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4131,10 +4137,10 @@
         <v>327</v>
       </c>
       <c r="D95" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E95" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4148,10 +4154,10 @@
         <v>328</v>
       </c>
       <c r="D96" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E96" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4182,10 +4188,10 @@
         <v>330</v>
       </c>
       <c r="D98" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E98" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4199,10 +4205,10 @@
         <v>331</v>
       </c>
       <c r="D99" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E99" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4233,10 +4239,10 @@
         <v>333</v>
       </c>
       <c r="D101" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E101" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4301,10 +4307,10 @@
         <v>337</v>
       </c>
       <c r="D105" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E105" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4318,7 +4324,7 @@
         <v>338</v>
       </c>
       <c r="D106" t="s">
-        <v>465</v>
+        <v>516</v>
       </c>
       <c r="E106" t="s">
         <v>463</v>
@@ -4352,10 +4358,10 @@
         <v>340</v>
       </c>
       <c r="D108" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E108" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4369,10 +4375,10 @@
         <v>341</v>
       </c>
       <c r="D109" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E109" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4386,10 +4392,10 @@
         <v>342</v>
       </c>
       <c r="D110" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E110" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4403,10 +4409,10 @@
         <v>343</v>
       </c>
       <c r="D111" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E111" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4420,10 +4426,10 @@
         <v>344</v>
       </c>
       <c r="D112" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E112" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4437,10 +4443,10 @@
         <v>345</v>
       </c>
       <c r="D113" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E113" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4454,10 +4460,10 @@
         <v>346</v>
       </c>
       <c r="D114" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E114" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4522,10 +4528,10 @@
         <v>350</v>
       </c>
       <c r="D118" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E118" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4539,10 +4545,10 @@
         <v>351</v>
       </c>
       <c r="D119" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E119" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4559,7 +4565,7 @@
         <v>463</v>
       </c>
       <c r="E120" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4590,10 +4596,10 @@
         <v>354</v>
       </c>
       <c r="D122" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="E122" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4607,10 +4613,10 @@
         <v>355</v>
       </c>
       <c r="D123" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E123" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4658,7 +4664,7 @@
         <v>358</v>
       </c>
       <c r="D126" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E126" t="s">
         <v>463</v>
@@ -4692,10 +4698,10 @@
         <v>360</v>
       </c>
       <c r="D128" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E128" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4709,10 +4715,10 @@
         <v>361</v>
       </c>
       <c r="D129" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E129" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4726,10 +4732,10 @@
         <v>362</v>
       </c>
       <c r="D130" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E130" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4743,10 +4749,10 @@
         <v>363</v>
       </c>
       <c r="D131" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="E131" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4777,10 +4783,10 @@
         <v>365</v>
       </c>
       <c r="D133" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E133" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4811,10 +4817,10 @@
         <v>367</v>
       </c>
       <c r="D135" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E135" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4828,10 +4834,10 @@
         <v>368</v>
       </c>
       <c r="D136" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="E136" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4845,10 +4851,10 @@
         <v>369</v>
       </c>
       <c r="D137" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E137" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4862,10 +4868,10 @@
         <v>370</v>
       </c>
       <c r="D138" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E138" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4879,10 +4885,10 @@
         <v>371</v>
       </c>
       <c r="D139" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E139" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4896,10 +4902,10 @@
         <v>372</v>
       </c>
       <c r="D140" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E140" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4913,10 +4919,10 @@
         <v>373</v>
       </c>
       <c r="D141" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E141" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -4930,10 +4936,10 @@
         <v>374</v>
       </c>
       <c r="D142" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E142" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -4950,7 +4956,7 @@
         <v>463</v>
       </c>
       <c r="E143" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -4981,10 +4987,10 @@
         <v>377</v>
       </c>
       <c r="D145" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E145" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4998,10 +5004,10 @@
         <v>378</v>
       </c>
       <c r="D146" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E146" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -5032,10 +5038,10 @@
         <v>380</v>
       </c>
       <c r="D148" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E148" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5049,10 +5055,10 @@
         <v>381</v>
       </c>
       <c r="D149" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E149" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5066,10 +5072,10 @@
         <v>382</v>
       </c>
       <c r="D150" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="E150" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5083,10 +5089,10 @@
         <v>383</v>
       </c>
       <c r="D151" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E151" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5100,10 +5106,10 @@
         <v>384</v>
       </c>
       <c r="D152" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E152" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5120,7 +5126,7 @@
         <v>463</v>
       </c>
       <c r="E153" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5134,10 +5140,10 @@
         <v>386</v>
       </c>
       <c r="D154" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E154" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5151,10 +5157,10 @@
         <v>387</v>
       </c>
       <c r="D155" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E155" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5202,10 +5208,10 @@
         <v>390</v>
       </c>
       <c r="D158" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E158" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5236,7 +5242,7 @@
         <v>392</v>
       </c>
       <c r="D160" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E160" t="s">
         <v>463</v>
@@ -5253,7 +5259,7 @@
         <v>393</v>
       </c>
       <c r="D161" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="E161" t="s">
         <v>463</v>
@@ -5270,10 +5276,10 @@
         <v>394</v>
       </c>
       <c r="D162" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E162" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5290,7 +5296,7 @@
         <v>463</v>
       </c>
       <c r="E163" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5338,10 +5344,10 @@
         <v>398</v>
       </c>
       <c r="D166" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="E166" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5355,10 +5361,10 @@
         <v>399</v>
       </c>
       <c r="D167" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E167" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5372,10 +5378,10 @@
         <v>400</v>
       </c>
       <c r="D168" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="E168" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5406,10 +5412,10 @@
         <v>402</v>
       </c>
       <c r="D170" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="E170" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5423,10 +5429,10 @@
         <v>403</v>
       </c>
       <c r="D171" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E171" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5440,10 +5446,10 @@
         <v>404</v>
       </c>
       <c r="D172" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="E172" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5457,10 +5463,10 @@
         <v>405</v>
       </c>
       <c r="D173" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="E173" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5474,10 +5480,10 @@
         <v>406</v>
       </c>
       <c r="D174" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="E174" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5491,10 +5497,10 @@
         <v>407</v>
       </c>
       <c r="D175" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E175" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5508,10 +5514,10 @@
         <v>408</v>
       </c>
       <c r="D176" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="E176" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5559,10 +5565,10 @@
         <v>411</v>
       </c>
       <c r="D179" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E179" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5576,10 +5582,10 @@
         <v>412</v>
       </c>
       <c r="D180" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="E180" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5593,10 +5599,10 @@
         <v>413</v>
       </c>
       <c r="D181" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E181" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5627,7 +5633,7 @@
         <v>415</v>
       </c>
       <c r="D183" t="s">
-        <v>463</v>
+        <v>510</v>
       </c>
       <c r="E183" t="s">
         <v>463</v>
@@ -5695,7 +5701,7 @@
         <v>419</v>
       </c>
       <c r="D187" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="E187" t="s">
         <v>463</v>
@@ -5729,10 +5735,10 @@
         <v>421</v>
       </c>
       <c r="D189" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E189" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5763,10 +5769,10 @@
         <v>423</v>
       </c>
       <c r="D191" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E191" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5780,10 +5786,10 @@
         <v>424</v>
       </c>
       <c r="D192" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="E192" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5814,7 +5820,7 @@
         <v>426</v>
       </c>
       <c r="D194" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="E194" t="s">
         <v>426</v>
@@ -5831,10 +5837,10 @@
         <v>427</v>
       </c>
       <c r="D195" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E195" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5848,10 +5854,10 @@
         <v>428</v>
       </c>
       <c r="D196" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="E196" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5902,7 +5908,7 @@
         <v>463</v>
       </c>
       <c r="E199" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -5916,10 +5922,10 @@
         <v>432</v>
       </c>
       <c r="D200" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E200" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5933,10 +5939,10 @@
         <v>433</v>
       </c>
       <c r="D201" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E201" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -5967,10 +5973,10 @@
         <v>435</v>
       </c>
       <c r="D203" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="E203" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -5984,7 +5990,7 @@
         <v>436</v>
       </c>
       <c r="D204" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E204" t="s">
         <v>436</v>
@@ -6035,10 +6041,10 @@
         <v>439</v>
       </c>
       <c r="D207" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="E207" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -6055,7 +6061,7 @@
         <v>463</v>
       </c>
       <c r="E208" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6069,10 +6075,10 @@
         <v>441</v>
       </c>
       <c r="D209" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="E209" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6086,10 +6092,10 @@
         <v>442</v>
       </c>
       <c r="D210" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E210" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6120,10 +6126,10 @@
         <v>444</v>
       </c>
       <c r="D212" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E212" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6157,7 +6163,7 @@
         <v>463</v>
       </c>
       <c r="E214" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6174,7 +6180,7 @@
         <v>463</v>
       </c>
       <c r="E215" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6205,10 +6211,10 @@
         <v>449</v>
       </c>
       <c r="D217" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E217" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6222,10 +6228,10 @@
         <v>450</v>
       </c>
       <c r="D218" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="E218" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6273,10 +6279,10 @@
         <v>453</v>
       </c>
       <c r="D221" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="E221" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6293,7 +6299,7 @@
         <v>454</v>
       </c>
       <c r="E222" t="s">
-        <v>706</v>
+        <v>463</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -6307,10 +6313,10 @@
         <v>455</v>
       </c>
       <c r="D223" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="E223" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -6324,10 +6330,10 @@
         <v>456</v>
       </c>
       <c r="D224" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="E224" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6358,10 +6364,10 @@
         <v>458</v>
       </c>
       <c r="D226" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E226" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6395,7 +6401,7 @@
         <v>463</v>
       </c>
       <c r="E228" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6409,7 +6415,7 @@
         <v>461</v>
       </c>
       <c r="D229" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="E229" t="s">
         <v>461</v>

</xml_diff>

<commit_message>
combine stats is working
</commit_message>
<xml_diff>
--- a/data/merge.xlsx
+++ b/data/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="800">
   <si>
     <t>Index</t>
   </si>
@@ -1408,7 +1408,7 @@
     <t>Kentucky</t>
   </si>
   <si>
-    <t>NC State</t>
+    <t>Ball St</t>
   </si>
   <si>
     <t>Liberty</t>
@@ -1435,7 +1435,7 @@
     <t>Kansas St</t>
   </si>
   <si>
-    <t>U Mass</t>
+    <t>Mississippi</t>
   </si>
   <si>
     <t>Oregon St</t>
@@ -1486,7 +1486,7 @@
     <t>Wake Forest</t>
   </si>
   <si>
-    <t>Ohio</t>
+    <t>?</t>
   </si>
   <si>
     <t>N Mex State</t>
@@ -1528,6 +1528,12 @@
     <t>Miss State</t>
   </si>
   <si>
+    <t>TX Christian</t>
+  </si>
+  <si>
+    <t>TX El Paso</t>
+  </si>
+  <si>
     <t>GA Tech</t>
   </si>
   <si>
@@ -1540,7 +1546,7 @@
     <t>LA Tech</t>
   </si>
   <si>
-    <t>S Methodist</t>
+    <t>Sam Hous St</t>
   </si>
   <si>
     <t>James Mad</t>
@@ -1558,9 +1564,6 @@
     <t>Kansas</t>
   </si>
   <si>
-    <t>Ball St</t>
-  </si>
-  <si>
     <t>Arkansas</t>
   </si>
   <si>
@@ -1570,9 +1573,6 @@
     <t>Washington</t>
   </si>
   <si>
-    <t>TX Christian</t>
-  </si>
-  <si>
     <t>Middle Tenn</t>
   </si>
   <si>
@@ -1594,9 +1594,6 @@
     <t>S Alabama</t>
   </si>
   <si>
-    <t>Sam Hous St</t>
-  </si>
-  <si>
     <t>Notre Dame</t>
   </si>
   <si>
@@ -1642,6 +1639,9 @@
     <t>Boston Col</t>
   </si>
   <si>
+    <t>Ohio St</t>
+  </si>
+  <si>
     <t>Buffalo</t>
   </si>
   <si>
@@ -1669,12 +1669,6 @@
     <t>Illinois</t>
   </si>
   <si>
-    <t>TX El Paso</t>
-  </si>
-  <si>
-    <t>Ohio St</t>
-  </si>
-  <si>
     <t>Wisconsin</t>
   </si>
   <si>
@@ -1691,9 +1685,6 @@
   </si>
   <si>
     <t>Arizona</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
   </si>
   <si>
     <t>Arkansas St</t>
@@ -2814,7 +2805,7 @@
         <v>234</v>
       </c>
       <c r="E2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2828,7 +2819,7 @@
         <v>235</v>
       </c>
       <c r="E3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2842,7 +2833,7 @@
         <v>236</v>
       </c>
       <c r="E4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2859,7 +2850,7 @@
         <v>463</v>
       </c>
       <c r="E5" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2873,7 +2864,7 @@
         <v>238</v>
       </c>
       <c r="E6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2890,7 +2881,7 @@
         <v>464</v>
       </c>
       <c r="E7" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2904,7 +2895,7 @@
         <v>240</v>
       </c>
       <c r="E8" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2921,7 +2912,7 @@
         <v>465</v>
       </c>
       <c r="E9" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2938,7 +2929,7 @@
         <v>466</v>
       </c>
       <c r="E10" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2952,7 +2943,7 @@
         <v>243</v>
       </c>
       <c r="E11" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2966,7 +2957,7 @@
         <v>244</v>
       </c>
       <c r="E12" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2980,7 +2971,7 @@
         <v>245</v>
       </c>
       <c r="E13" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2997,7 +2988,7 @@
         <v>467</v>
       </c>
       <c r="E14" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3011,7 +3002,7 @@
         <v>247</v>
       </c>
       <c r="E15" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3028,7 +3019,7 @@
         <v>468</v>
       </c>
       <c r="E16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3045,7 +3036,7 @@
         <v>249</v>
       </c>
       <c r="E17" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3059,7 +3050,7 @@
         <v>250</v>
       </c>
       <c r="E18" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3076,7 +3067,7 @@
         <v>469</v>
       </c>
       <c r="E19" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3090,7 +3081,7 @@
         <v>252</v>
       </c>
       <c r="E20" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3104,7 +3095,7 @@
         <v>253</v>
       </c>
       <c r="E21" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3118,7 +3109,7 @@
         <v>254</v>
       </c>
       <c r="E22" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3135,7 +3126,7 @@
         <v>470</v>
       </c>
       <c r="E23" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3152,7 +3143,7 @@
         <v>471</v>
       </c>
       <c r="E24" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3169,7 +3160,7 @@
         <v>472</v>
       </c>
       <c r="E25" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3183,7 +3174,7 @@
         <v>258</v>
       </c>
       <c r="E26" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3200,7 +3191,7 @@
         <v>473</v>
       </c>
       <c r="E27" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3217,7 +3208,7 @@
         <v>474</v>
       </c>
       <c r="E28" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3231,7 +3222,7 @@
         <v>261</v>
       </c>
       <c r="E29" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3245,7 +3236,7 @@
         <v>262</v>
       </c>
       <c r="E30" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3262,7 +3253,7 @@
         <v>475</v>
       </c>
       <c r="E31" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3276,7 +3267,7 @@
         <v>264</v>
       </c>
       <c r="E32" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3293,7 +3284,7 @@
         <v>476</v>
       </c>
       <c r="E33" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3310,7 +3301,7 @@
         <v>477</v>
       </c>
       <c r="E34" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3327,7 +3318,7 @@
         <v>478</v>
       </c>
       <c r="E35" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3344,7 +3335,7 @@
         <v>479</v>
       </c>
       <c r="E36" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3358,7 +3349,7 @@
         <v>269</v>
       </c>
       <c r="E37" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3375,7 +3366,7 @@
         <v>270</v>
       </c>
       <c r="E38" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3389,7 +3380,7 @@
         <v>271</v>
       </c>
       <c r="E39" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3406,7 +3397,7 @@
         <v>480</v>
       </c>
       <c r="E40" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3420,7 +3411,7 @@
         <v>273</v>
       </c>
       <c r="E41" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3434,7 +3425,7 @@
         <v>274</v>
       </c>
       <c r="E42" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3448,7 +3439,7 @@
         <v>275</v>
       </c>
       <c r="E43" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3462,7 +3453,7 @@
         <v>276</v>
       </c>
       <c r="E44" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3479,7 +3470,7 @@
         <v>481</v>
       </c>
       <c r="E45" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3493,7 +3484,7 @@
         <v>278</v>
       </c>
       <c r="E46" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3510,7 +3501,7 @@
         <v>279</v>
       </c>
       <c r="E47" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -3524,7 +3515,7 @@
         <v>280</v>
       </c>
       <c r="E48" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3538,7 +3529,7 @@
         <v>281</v>
       </c>
       <c r="E49" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3569,7 +3560,7 @@
         <v>483</v>
       </c>
       <c r="E51" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3583,7 +3574,7 @@
         <v>284</v>
       </c>
       <c r="E52" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3600,7 +3591,7 @@
         <v>484</v>
       </c>
       <c r="E53" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3617,7 +3608,7 @@
         <v>485</v>
       </c>
       <c r="E54" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3648,7 +3639,7 @@
         <v>288</v>
       </c>
       <c r="E56" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3665,7 +3656,7 @@
         <v>487</v>
       </c>
       <c r="E57" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3682,7 +3673,7 @@
         <v>488</v>
       </c>
       <c r="E58" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3699,7 +3690,7 @@
         <v>489</v>
       </c>
       <c r="E59" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3716,7 +3707,7 @@
         <v>490</v>
       </c>
       <c r="E60" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3733,7 +3724,7 @@
         <v>491</v>
       </c>
       <c r="E61" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3750,7 +3741,7 @@
         <v>492</v>
       </c>
       <c r="E62" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3767,7 +3758,7 @@
         <v>493</v>
       </c>
       <c r="E63" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3784,7 +3775,7 @@
         <v>494</v>
       </c>
       <c r="E64" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3798,7 +3789,7 @@
         <v>297</v>
       </c>
       <c r="E65" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3815,7 +3806,7 @@
         <v>495</v>
       </c>
       <c r="E66" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3829,7 +3820,7 @@
         <v>299</v>
       </c>
       <c r="E67" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3846,7 +3837,7 @@
         <v>496</v>
       </c>
       <c r="E68" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3860,7 +3851,7 @@
         <v>301</v>
       </c>
       <c r="E69" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3891,7 +3882,7 @@
         <v>303</v>
       </c>
       <c r="E71" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3905,7 +3896,7 @@
         <v>304</v>
       </c>
       <c r="E72" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3922,7 +3913,7 @@
         <v>498</v>
       </c>
       <c r="E73" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3939,7 +3930,7 @@
         <v>499</v>
       </c>
       <c r="E74" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3953,7 +3944,7 @@
         <v>307</v>
       </c>
       <c r="E75" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3984,7 +3975,7 @@
         <v>309</v>
       </c>
       <c r="E77" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3998,7 +3989,7 @@
         <v>310</v>
       </c>
       <c r="E78" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4015,7 +4006,7 @@
         <v>501</v>
       </c>
       <c r="E79" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -4029,7 +4020,7 @@
         <v>312</v>
       </c>
       <c r="E80" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -4043,7 +4034,7 @@
         <v>313</v>
       </c>
       <c r="E81" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -4060,7 +4051,7 @@
         <v>502</v>
       </c>
       <c r="E82" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -4077,7 +4068,7 @@
         <v>503</v>
       </c>
       <c r="E83" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -4101,8 +4092,11 @@
       <c r="C85" t="s">
         <v>317</v>
       </c>
+      <c r="D85" t="s">
+        <v>504</v>
+      </c>
       <c r="E85" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -4115,8 +4109,11 @@
       <c r="C86" t="s">
         <v>318</v>
       </c>
+      <c r="D86" t="s">
+        <v>505</v>
+      </c>
       <c r="E86" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -4130,7 +4127,7 @@
         <v>319</v>
       </c>
       <c r="E87" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -4144,7 +4141,7 @@
         <v>320</v>
       </c>
       <c r="E88" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4158,7 +4155,7 @@
         <v>321</v>
       </c>
       <c r="E89" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4172,7 +4169,7 @@
         <v>322</v>
       </c>
       <c r="E90" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4186,10 +4183,10 @@
         <v>323</v>
       </c>
       <c r="D91" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E91" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4203,10 +4200,10 @@
         <v>324</v>
       </c>
       <c r="D92" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E92" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4220,10 +4217,10 @@
         <v>325</v>
       </c>
       <c r="D93" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E93" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -4237,10 +4234,10 @@
         <v>326</v>
       </c>
       <c r="D94" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E94" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4254,10 +4251,10 @@
         <v>327</v>
       </c>
       <c r="D95" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E95" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4271,10 +4268,10 @@
         <v>328</v>
       </c>
       <c r="D96" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E96" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4288,7 +4285,7 @@
         <v>329</v>
       </c>
       <c r="E97" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4302,10 +4299,10 @@
         <v>330</v>
       </c>
       <c r="D98" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E98" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4319,10 +4316,10 @@
         <v>331</v>
       </c>
       <c r="D99" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E99" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4336,7 +4333,7 @@
         <v>332</v>
       </c>
       <c r="E100" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4350,10 +4347,10 @@
         <v>333</v>
       </c>
       <c r="D101" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E101" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4367,7 +4364,7 @@
         <v>334</v>
       </c>
       <c r="E102" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4384,7 +4381,7 @@
         <v>335</v>
       </c>
       <c r="E103" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -4398,7 +4395,7 @@
         <v>336</v>
       </c>
       <c r="E104" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4412,10 +4409,10 @@
         <v>337</v>
       </c>
       <c r="D105" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E105" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4429,10 +4426,10 @@
         <v>338</v>
       </c>
       <c r="D106" t="s">
-        <v>514</v>
+        <v>490</v>
       </c>
       <c r="E106" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4449,7 +4446,7 @@
         <v>339</v>
       </c>
       <c r="E107" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -4463,10 +4460,10 @@
         <v>340</v>
       </c>
       <c r="D108" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E108" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4480,10 +4477,10 @@
         <v>341</v>
       </c>
       <c r="D109" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E109" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4497,10 +4494,10 @@
         <v>342</v>
       </c>
       <c r="D110" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E110" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4514,10 +4511,10 @@
         <v>343</v>
       </c>
       <c r="D111" t="s">
-        <v>518</v>
+        <v>490</v>
       </c>
       <c r="E111" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4534,7 +4531,7 @@
         <v>519</v>
       </c>
       <c r="E112" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4551,7 +4548,7 @@
         <v>520</v>
       </c>
       <c r="E113" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4568,7 +4565,7 @@
         <v>521</v>
       </c>
       <c r="E114" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4582,7 +4579,7 @@
         <v>347</v>
       </c>
       <c r="E115" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4596,7 +4593,7 @@
         <v>348</v>
       </c>
       <c r="E116" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4610,7 +4607,7 @@
         <v>349</v>
       </c>
       <c r="E117" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4627,7 +4624,7 @@
         <v>522</v>
       </c>
       <c r="E118" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4644,7 +4641,7 @@
         <v>523</v>
       </c>
       <c r="E119" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4658,7 +4655,7 @@
         <v>352</v>
       </c>
       <c r="E120" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4672,7 +4669,7 @@
         <v>353</v>
       </c>
       <c r="E121" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4689,7 +4686,7 @@
         <v>524</v>
       </c>
       <c r="E122" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4706,7 +4703,7 @@
         <v>525</v>
       </c>
       <c r="E123" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4720,7 +4717,7 @@
         <v>356</v>
       </c>
       <c r="E124" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4734,7 +4731,7 @@
         <v>357</v>
       </c>
       <c r="E125" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4748,7 +4745,7 @@
         <v>358</v>
       </c>
       <c r="D126" t="s">
-        <v>526</v>
+        <v>490</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4762,7 +4759,7 @@
         <v>359</v>
       </c>
       <c r="E127" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -4776,10 +4773,10 @@
         <v>360</v>
       </c>
       <c r="D128" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E128" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4793,10 +4790,10 @@
         <v>361</v>
       </c>
       <c r="D129" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E129" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4810,10 +4807,10 @@
         <v>362</v>
       </c>
       <c r="D130" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E130" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4827,10 +4824,10 @@
         <v>363</v>
       </c>
       <c r="D131" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E131" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4844,7 +4841,7 @@
         <v>364</v>
       </c>
       <c r="E132" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -4858,10 +4855,10 @@
         <v>365</v>
       </c>
       <c r="D133" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E133" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4886,10 +4883,10 @@
         <v>367</v>
       </c>
       <c r="D135" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E135" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4903,10 +4900,10 @@
         <v>368</v>
       </c>
       <c r="D136" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E136" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4920,10 +4917,10 @@
         <v>369</v>
       </c>
       <c r="D137" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E137" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4937,10 +4934,10 @@
         <v>370</v>
       </c>
       <c r="D138" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E138" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4954,10 +4951,10 @@
         <v>371</v>
       </c>
       <c r="D139" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E139" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4971,10 +4968,10 @@
         <v>372</v>
       </c>
       <c r="D140" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E140" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4988,10 +4985,10 @@
         <v>373</v>
       </c>
       <c r="D141" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E141" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -5005,10 +5002,10 @@
         <v>374</v>
       </c>
       <c r="D142" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E142" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -5022,7 +5019,7 @@
         <v>375</v>
       </c>
       <c r="E143" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -5047,10 +5044,10 @@
         <v>377</v>
       </c>
       <c r="D145" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E145" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -5064,10 +5061,10 @@
         <v>378</v>
       </c>
       <c r="D146" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E146" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -5080,8 +5077,11 @@
       <c r="C147" t="s">
         <v>379</v>
       </c>
+      <c r="D147" t="s">
+        <v>541</v>
+      </c>
       <c r="E147" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -5098,7 +5098,7 @@
         <v>542</v>
       </c>
       <c r="E148" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5115,7 +5115,7 @@
         <v>543</v>
       </c>
       <c r="E149" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5132,7 +5132,7 @@
         <v>544</v>
       </c>
       <c r="E150" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5149,7 +5149,7 @@
         <v>545</v>
       </c>
       <c r="E151" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5166,7 +5166,7 @@
         <v>546</v>
       </c>
       <c r="E152" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5179,8 +5179,11 @@
       <c r="C153" t="s">
         <v>385</v>
       </c>
+      <c r="D153" t="s">
+        <v>487</v>
+      </c>
       <c r="E153" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5197,7 +5200,7 @@
         <v>547</v>
       </c>
       <c r="E154" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5214,7 +5217,7 @@
         <v>548</v>
       </c>
       <c r="E155" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5228,7 +5231,7 @@
         <v>388</v>
       </c>
       <c r="E156" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5245,7 +5248,7 @@
         <v>389</v>
       </c>
       <c r="E157" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5262,7 +5265,7 @@
         <v>549</v>
       </c>
       <c r="E158" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5276,7 +5279,7 @@
         <v>391</v>
       </c>
       <c r="E159" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5293,7 +5296,7 @@
         <v>550</v>
       </c>
       <c r="E160" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -5307,10 +5310,10 @@
         <v>393</v>
       </c>
       <c r="D161" t="s">
-        <v>551</v>
+        <v>490</v>
       </c>
       <c r="E161" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -5324,10 +5327,10 @@
         <v>394</v>
       </c>
       <c r="D162" t="s">
-        <v>552</v>
+        <v>490</v>
       </c>
       <c r="E162" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5341,7 +5344,7 @@
         <v>395</v>
       </c>
       <c r="E163" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5369,7 +5372,7 @@
         <v>397</v>
       </c>
       <c r="E165" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5383,10 +5386,10 @@
         <v>398</v>
       </c>
       <c r="D166" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E166" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5400,10 +5403,10 @@
         <v>399</v>
       </c>
       <c r="D167" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E167" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5417,10 +5420,10 @@
         <v>400</v>
       </c>
       <c r="D168" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E168" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5434,7 +5437,7 @@
         <v>401</v>
       </c>
       <c r="E169" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -5448,10 +5451,10 @@
         <v>402</v>
       </c>
       <c r="D170" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E170" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5465,10 +5468,10 @@
         <v>403</v>
       </c>
       <c r="D171" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E171" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5482,10 +5485,10 @@
         <v>404</v>
       </c>
       <c r="D172" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E172" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5499,10 +5502,10 @@
         <v>405</v>
       </c>
       <c r="D173" t="s">
-        <v>559</v>
+        <v>503</v>
       </c>
       <c r="E173" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5516,10 +5519,10 @@
         <v>406</v>
       </c>
       <c r="D174" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E174" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5533,10 +5536,10 @@
         <v>407</v>
       </c>
       <c r="D175" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E175" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5550,10 +5553,10 @@
         <v>408</v>
       </c>
       <c r="D176" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E176" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5567,7 +5570,7 @@
         <v>409</v>
       </c>
       <c r="E177" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -5581,7 +5584,7 @@
         <v>410</v>
       </c>
       <c r="E178" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -5595,10 +5598,10 @@
         <v>411</v>
       </c>
       <c r="D179" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E179" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5612,10 +5615,10 @@
         <v>412</v>
       </c>
       <c r="D180" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E180" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5629,10 +5632,10 @@
         <v>413</v>
       </c>
       <c r="D181" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E181" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5646,7 +5649,7 @@
         <v>414</v>
       </c>
       <c r="E182" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5660,7 +5663,7 @@
         <v>415</v>
       </c>
       <c r="E183" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -5674,7 +5677,7 @@
         <v>416</v>
       </c>
       <c r="E184" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -5688,7 +5691,7 @@
         <v>417</v>
       </c>
       <c r="E185" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -5702,7 +5705,7 @@
         <v>418</v>
       </c>
       <c r="E186" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -5716,10 +5719,10 @@
         <v>419</v>
       </c>
       <c r="D187" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E187" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5733,7 +5736,7 @@
         <v>420</v>
       </c>
       <c r="E188" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5747,10 +5750,10 @@
         <v>421</v>
       </c>
       <c r="D189" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E189" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5764,7 +5767,7 @@
         <v>422</v>
       </c>
       <c r="E190" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -5778,10 +5781,10 @@
         <v>423</v>
       </c>
       <c r="D191" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E191" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5795,10 +5798,10 @@
         <v>424</v>
       </c>
       <c r="D192" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E192" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5812,7 +5815,7 @@
         <v>425</v>
       </c>
       <c r="E193" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -5826,7 +5829,7 @@
         <v>426</v>
       </c>
       <c r="D194" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E194" t="s">
         <v>426</v>
@@ -5843,10 +5846,10 @@
         <v>427</v>
       </c>
       <c r="D195" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E195" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5860,10 +5863,10 @@
         <v>428</v>
       </c>
       <c r="D196" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E196" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5877,7 +5880,7 @@
         <v>429</v>
       </c>
       <c r="E197" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -5894,7 +5897,7 @@
         <v>430</v>
       </c>
       <c r="E198" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -5907,8 +5910,11 @@
       <c r="C199" t="s">
         <v>431</v>
       </c>
+      <c r="D199" t="s">
+        <v>496</v>
+      </c>
       <c r="E199" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -5922,10 +5928,10 @@
         <v>432</v>
       </c>
       <c r="D200" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E200" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5939,10 +5945,10 @@
         <v>433</v>
       </c>
       <c r="D201" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E201" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -5956,7 +5962,7 @@
         <v>434</v>
       </c>
       <c r="E202" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -5970,10 +5976,10 @@
         <v>435</v>
       </c>
       <c r="D203" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E203" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -5987,7 +5993,7 @@
         <v>436</v>
       </c>
       <c r="D204" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E204" t="s">
         <v>436</v>
@@ -6004,7 +6010,7 @@
         <v>437</v>
       </c>
       <c r="E205" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -6018,7 +6024,7 @@
         <v>438</v>
       </c>
       <c r="E206" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -6032,10 +6038,10 @@
         <v>439</v>
       </c>
       <c r="D207" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E207" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -6049,7 +6055,7 @@
         <v>440</v>
       </c>
       <c r="E208" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6063,10 +6069,10 @@
         <v>441</v>
       </c>
       <c r="D209" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E209" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6080,10 +6086,10 @@
         <v>442</v>
       </c>
       <c r="D210" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E210" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6097,7 +6103,7 @@
         <v>443</v>
       </c>
       <c r="E211" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -6111,10 +6117,10 @@
         <v>444</v>
       </c>
       <c r="D212" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E212" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6128,7 +6134,7 @@
         <v>445</v>
       </c>
       <c r="E213" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6142,7 +6148,7 @@
         <v>446</v>
       </c>
       <c r="E214" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6156,7 +6162,7 @@
         <v>447</v>
       </c>
       <c r="E215" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6170,7 +6176,7 @@
         <v>448</v>
       </c>
       <c r="E216" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6184,10 +6190,10 @@
         <v>449</v>
       </c>
       <c r="D217" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E217" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6201,10 +6207,10 @@
         <v>450</v>
       </c>
       <c r="D218" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E218" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6218,7 +6224,7 @@
         <v>451</v>
       </c>
       <c r="E219" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -6232,7 +6238,7 @@
         <v>452</v>
       </c>
       <c r="E220" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -6246,10 +6252,10 @@
         <v>453</v>
       </c>
       <c r="D221" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E221" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6266,7 +6272,7 @@
         <v>454</v>
       </c>
       <c r="E222" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -6280,10 +6286,10 @@
         <v>455</v>
       </c>
       <c r="D223" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E223" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -6297,10 +6303,10 @@
         <v>456</v>
       </c>
       <c r="D224" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E224" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6314,7 +6320,7 @@
         <v>457</v>
       </c>
       <c r="E225" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -6328,10 +6334,10 @@
         <v>458</v>
       </c>
       <c r="D226" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E226" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6345,7 +6351,7 @@
         <v>459</v>
       </c>
       <c r="E227" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -6359,7 +6365,7 @@
         <v>460</v>
       </c>
       <c r="E228" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6373,7 +6379,7 @@
         <v>461</v>
       </c>
       <c r="D229" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E229" t="s">
         <v>461</v>
@@ -6390,7 +6396,7 @@
         <v>462</v>
       </c>
       <c r="E230" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed None, empty columns
</commit_message>
<xml_diff>
--- a/data/merge.xlsx
+++ b/data/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="797">
   <si>
     <t>Index</t>
   </si>
@@ -1408,351 +1408,339 @@
     <t>Kentucky</t>
   </si>
   <si>
+    <t>Ball St</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>W Kentucky</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Florida St</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Kansas St</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Oregon St</t>
+  </si>
+  <si>
+    <t>Georgia St</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>S Florida</t>
+  </si>
+  <si>
+    <t>Fresno St</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>N Carolina</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>Penn St</t>
+  </si>
+  <si>
+    <t>Akron</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Wake Forest</t>
+  </si>
+  <si>
+    <t>N Mex State</t>
+  </si>
+  <si>
+    <t>Wash State</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>San Diego St</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
     <t>NC State</t>
   </si>
   <si>
-    <t>Liberty</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Colorado St</t>
   </si>
   <si>
     <t>W Virginia</t>
   </si>
   <si>
-    <t>W Kentucky</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Florida St</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Kansas St</t>
-  </si>
-  <si>
-    <t>U Mass</t>
-  </si>
-  <si>
-    <t>Oregon St</t>
-  </si>
-  <si>
-    <t>Georgia St</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>S Florida</t>
-  </si>
-  <si>
-    <t>Fresno St</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>N Carolina</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Cincinnati</t>
-  </si>
-  <si>
-    <t>Penn St</t>
-  </si>
-  <si>
-    <t>Akron</t>
-  </si>
-  <si>
-    <t>Duke</t>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>TX Christian</t>
+  </si>
+  <si>
+    <t>TX El Paso</t>
+  </si>
+  <si>
+    <t>GA Tech</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>UL Monroe</t>
+  </si>
+  <si>
+    <t>LA Tech</t>
+  </si>
+  <si>
+    <t>Sam Hous St</t>
+  </si>
+  <si>
+    <t>James Mad</t>
+  </si>
+  <si>
+    <t>E Michigan</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Oklahoma St</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Middle Tenn</t>
+  </si>
+  <si>
+    <t>Kent St</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>S Alabama</t>
+  </si>
+  <si>
+    <t>Notre Dame</t>
+  </si>
+  <si>
+    <t>Coastal Car</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Texas St</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>Fla Atlantic</t>
+  </si>
+  <si>
+    <t>Bowling Grn</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>Texas Tech</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Michigan St</t>
+  </si>
+  <si>
+    <t>Boston Col</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Purdue</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M</t>
+  </si>
+  <si>
+    <t>Jksnville St</t>
   </si>
   <si>
     <t>VA Tech</t>
   </si>
   <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Wake Forest</t>
+    <t>Old Dominion</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Central Mich</t>
   </si>
   <si>
     <t>Ohio</t>
   </si>
   <si>
-    <t>N Mex State</t>
-  </si>
-  <si>
-    <t>Wash State</t>
-  </si>
-  <si>
-    <t>Louisville</t>
-  </si>
-  <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
-    <t>San Diego St</t>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>E Carolina</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Iowa St</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Miss State</t>
+  </si>
+  <si>
+    <t>Arkansas St</t>
+  </si>
+  <si>
+    <t>W Michigan</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>GA Southern</t>
+  </si>
+  <si>
+    <t>Baylor</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Boise St</t>
+  </si>
+  <si>
+    <t>S Mississippi</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Arizona St</t>
+  </si>
+  <si>
+    <t>Marshall</t>
   </si>
   <si>
     <t>App State</t>
   </si>
   <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Colorado St</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Army</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Miss State</t>
-  </si>
-  <si>
-    <t>GA Tech</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>UL Monroe</t>
-  </si>
-  <si>
-    <t>LA Tech</t>
-  </si>
-  <si>
-    <t>S Methodist</t>
-  </si>
-  <si>
-    <t>James Mad</t>
-  </si>
-  <si>
-    <t>E Michigan</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Oklahoma St</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Ball St</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
+    <t>North Texas</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Tulane</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>Florida Intl</t>
   </si>
   <si>
     <t>Florida</t>
   </si>
   <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>TX Christian</t>
-  </si>
-  <si>
-    <t>Middle Tenn</t>
-  </si>
-  <si>
-    <t>Kent St</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Temple</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Stanford</t>
-  </si>
-  <si>
-    <t>S Alabama</t>
-  </si>
-  <si>
-    <t>Sam Hous St</t>
-  </si>
-  <si>
-    <t>Notre Dame</t>
-  </si>
-  <si>
-    <t>Coastal Car</t>
-  </si>
-  <si>
-    <t>Syracuse</t>
-  </si>
-  <si>
-    <t>Texas St</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Auburn</t>
-  </si>
-  <si>
-    <t>Fla Atlantic</t>
-  </si>
-  <si>
-    <t>Bowling Grn</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>N Illinois</t>
-  </si>
-  <si>
-    <t>Northwestern</t>
-  </si>
-  <si>
-    <t>Texas Tech</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Michigan St</t>
-  </si>
-  <si>
-    <t>Boston Col</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Purdue</t>
-  </si>
-  <si>
-    <t>Texas A&amp;M</t>
-  </si>
-  <si>
-    <t>Jksnville St</t>
-  </si>
-  <si>
-    <t>Old Dominion</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Central Mich</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>TX El Paso</t>
-  </si>
-  <si>
-    <t>Ohio St</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>E Carolina</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Iowa St</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Arkansas St</t>
-  </si>
-  <si>
-    <t>W Michigan</t>
-  </si>
-  <si>
-    <t>Toledo</t>
-  </si>
-  <si>
-    <t>Tulsa</t>
-  </si>
-  <si>
-    <t>GA Southern</t>
-  </si>
-  <si>
-    <t>Baylor</t>
-  </si>
-  <si>
-    <t>Troy</t>
-  </si>
-  <si>
-    <t>Boise St</t>
-  </si>
-  <si>
-    <t>S Mississippi</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Arizona St</t>
-  </si>
-  <si>
-    <t>Marshall</t>
-  </si>
-  <si>
-    <t>North Texas</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>Tulane</t>
-  </si>
-  <si>
-    <t>Navy</t>
-  </si>
-  <si>
-    <t>Florida Intl</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
     <t>Rutgers</t>
   </si>
   <si>
@@ -1780,385 +1768,643 @@
     <t>Iowa</t>
   </si>
   <si>
+    <t>SOUTH CAROLINA STATE</t>
+  </si>
+  <si>
+    <t>DELAWARE STATE</t>
+  </si>
+  <si>
+    <t>CHATTANOOGA-TENNESSEE</t>
+  </si>
+  <si>
     <t>KENTUCKY</t>
   </si>
   <si>
+    <t>CHARLESTON SOUTHERN</t>
+  </si>
+  <si>
     <t>BALL STATE</t>
   </si>
   <si>
+    <t>S.F.AUSTIN</t>
+  </si>
+  <si>
     <t>LIBERTY</t>
   </si>
   <si>
+    <t>STONY BROOK</t>
+  </si>
+  <si>
+    <t>SOUTHERN ILLINOIS</t>
+  </si>
+  <si>
+    <t>SOUTH DAKOTA</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>RICHMOND</t>
+  </si>
+  <si>
+    <t>WESTERN KENTUCKY</t>
+  </si>
+  <si>
+    <t>SOUTHERN CALIFORNIA</t>
+  </si>
+  <si>
+    <t>WOFFORD</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>HOWARD</t>
+  </si>
+  <si>
+    <t>MAINE</t>
+  </si>
+  <si>
+    <t>SAMFORD</t>
+  </si>
+  <si>
+    <t>FLORIDA STATE</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>KANSAS STATE</t>
+  </si>
+  <si>
+    <t>YOUNGSTOWN STATE</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>OREGON STATE</t>
+  </si>
+  <si>
+    <t>BETHUNE-COOKMAN</t>
+  </si>
+  <si>
+    <t>NORFOLK STATE</t>
+  </si>
+  <si>
+    <t>GEORGIA STATE</t>
+  </si>
+  <si>
+    <t>NORTHERN ARIZONA</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>SOUTH FLORIDA</t>
+  </si>
+  <si>
+    <t>FRESNO STATE</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>CAMPBELL</t>
+  </si>
+  <si>
+    <t>TEXAS-SAN ANTONIO</t>
+  </si>
+  <si>
+    <t>BRYANT COLLEGE</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA A&amp;T</t>
+  </si>
+  <si>
+    <t>SOUTH EASTERN MISSOURI</t>
+  </si>
+  <si>
+    <t>NORTHERN IOWA</t>
+  </si>
+  <si>
+    <t>TOWSON</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>SACRED HEART</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>ALABAMA A&amp;M</t>
+  </si>
+  <si>
+    <t>SOUTHERN UTAH</t>
+  </si>
+  <si>
+    <t>CINCINNATI</t>
+  </si>
+  <si>
+    <t>INDIANA STATE</t>
+  </si>
+  <si>
+    <t>PENN STATE</t>
+  </si>
+  <si>
+    <t>AKRON</t>
+  </si>
+  <si>
+    <t>LAFAYETTE</t>
+  </si>
+  <si>
+    <t>UTAH TECH</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>WAKE FOREST</t>
+  </si>
+  <si>
+    <t>IDAHO</t>
+  </si>
+  <si>
+    <t>NEW MEXICO STATE</t>
+  </si>
+  <si>
+    <t>WASHINGTON STATE</t>
+  </si>
+  <si>
+    <t>LOUISVILLE</t>
+  </si>
+  <si>
+    <t>PITTSBURGH</t>
+  </si>
+  <si>
+    <t>ST.FRANCIS-PA</t>
+  </si>
+  <si>
+    <t>SAN DIEGO STATE</t>
+  </si>
+  <si>
     <t>CONNECTICUT</t>
   </si>
   <si>
-    <t>VIRGINIA</t>
-  </si>
-  <si>
-    <t>COLORADO</t>
-  </si>
-  <si>
-    <t>WAKE FOREST</t>
+    <t>NO. CAROLINA STATE</t>
+  </si>
+  <si>
+    <t>AUSTIN PEAY</t>
+  </si>
+  <si>
+    <t>EASTERN WASHINGTON</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>COLORADO STATE</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>MERRIMACK</t>
+  </si>
+  <si>
+    <t>TEXAS SOUTHERN</t>
+  </si>
+  <si>
+    <t>MCNEESE STATE</t>
+  </si>
+  <si>
+    <t>HOUSTON</t>
+  </si>
+  <si>
+    <t>JACKSON STATE</t>
+  </si>
+  <si>
+    <t>MORGAN STATE</t>
+  </si>
+  <si>
+    <t>MEMPHIS</t>
+  </si>
+  <si>
+    <t>MISSOURI STATE</t>
+  </si>
+  <si>
+    <t>TEXAS CHRISTIAN</t>
+  </si>
+  <si>
+    <t>TEXAS-EL PASO</t>
+  </si>
+  <si>
+    <t>MERCHANT MARINE</t>
+  </si>
+  <si>
+    <t>COLGATE</t>
+  </si>
+  <si>
+    <t>GARDNER-WEBB</t>
+  </si>
+  <si>
+    <t>WILLIAM &amp; MARY</t>
+  </si>
+  <si>
+    <t>GEORGIA TECH</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>LA - MONROE</t>
+  </si>
+  <si>
+    <t>LOUISIANA TECH</t>
+  </si>
+  <si>
+    <t>SAM HOUSTON</t>
+  </si>
+  <si>
+    <t>JAMES MADISON</t>
+  </si>
+  <si>
+    <t>NEW HAMPSHIRE</t>
+  </si>
+  <si>
+    <t>EASTERN MICHIGAN</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>PINE BLUFF-ARKANSAS</t>
+  </si>
+  <si>
+    <t>OKLAHOMA STATE</t>
+  </si>
+  <si>
+    <t>KENNESAW STATE</t>
+  </si>
+  <si>
+    <t>NEVADA-LAS VEGAS</t>
+  </si>
+  <si>
+    <t>MONMOUTH-NJ</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>FORT VALLEY STATE</t>
+  </si>
+  <si>
+    <t>U.C.L.A.</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>FLORIDA A&amp;M</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>ABILENE CHRISTIAN</t>
+  </si>
+  <si>
+    <t>MIDDLE TENNESSEE STATE</t>
+  </si>
+  <si>
+    <t>KENT STATE</t>
+  </si>
+  <si>
+    <t>WYOMING</t>
+  </si>
+  <si>
+    <t>TENNESSEE STATE</t>
+  </si>
+  <si>
+    <t>EAST TENNESSEE STATE</t>
+  </si>
+  <si>
+    <t>TEMPLE</t>
+  </si>
+  <si>
+    <t>MIAMI-FL</t>
+  </si>
+  <si>
+    <t>CENTRAL ARKANSAS</t>
+  </si>
+  <si>
+    <t>TENNESSEE TECH</t>
+  </si>
+  <si>
+    <t>STANFORD</t>
+  </si>
+  <si>
+    <t>SOUTH ALABAMA</t>
+  </si>
+  <si>
+    <t>CAL-DAVIS</t>
+  </si>
+  <si>
+    <t>NICHOLS</t>
+  </si>
+  <si>
+    <t>DUQUESNE</t>
+  </si>
+  <si>
+    <t>NOTRE DAME</t>
+  </si>
+  <si>
+    <t>COASTAL CAROLINA</t>
+  </si>
+  <si>
+    <t>SYRACUSE</t>
+  </si>
+  <si>
+    <t>TEXAS STATE-SAN MARCOS</t>
+  </si>
+  <si>
+    <t>WEBER STATE</t>
+  </si>
+  <si>
+    <t>ALABAMA</t>
+  </si>
+  <si>
+    <t>AUBURN</t>
   </si>
   <si>
     <t>FLORIDA ATLANTIC</t>
   </si>
   <si>
-    <t>OREGON</t>
-  </si>
-  <si>
-    <t>KANSAS STATE</t>
-  </si>
-  <si>
-    <t>OREGON STATE</t>
-  </si>
-  <si>
-    <t>TEXAS-SAN ANTONIO</t>
-  </si>
-  <si>
-    <t>FLORIDA STATE</t>
-  </si>
-  <si>
-    <t>NEW MEXICO</t>
-  </si>
-  <si>
-    <t>SOUTH FLORIDA</t>
-  </si>
-  <si>
-    <t>FRESNO STATE</t>
-  </si>
-  <si>
-    <t>OKLAHOMA</t>
-  </si>
-  <si>
-    <t>NO. CAROLINA STATE</t>
+    <t>BOWLING GREEN</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>NORTHWESTERN</t>
+  </si>
+  <si>
+    <t>TEXAS TECH</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>SO. EAST LOUISIANA</t>
+  </si>
+  <si>
+    <t>MICHIGAN STATE</t>
+  </si>
+  <si>
+    <t>BOSTON COLLEGE</t>
+  </si>
+  <si>
+    <t>BUFFALO</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>PURDUE</t>
+  </si>
+  <si>
+    <t>TEXAS A&amp;M</t>
+  </si>
+  <si>
+    <t>JACKSONVILLE STATE</t>
+  </si>
+  <si>
+    <t>VIRGINIA TECH</t>
+  </si>
+  <si>
+    <t>OLD DOMINION</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>WAGNER</t>
+  </si>
+  <si>
+    <t>BRIGHAM YOUNG</t>
+  </si>
+  <si>
+    <t>CENTRAL CONNECTICUT ST.</t>
+  </si>
+  <si>
+    <t>THE CITADEL</t>
+  </si>
+  <si>
+    <t>EASTERN ILLINOIS</t>
+  </si>
+  <si>
+    <t>CAL-POLY (SAN LOUIS OBISPO)</t>
+  </si>
+  <si>
+    <t>OHIO UNIV.</t>
+  </si>
+  <si>
+    <t>MURRAY STATE</t>
+  </si>
+  <si>
+    <t>NORTHERN COLORADO</t>
+  </si>
+  <si>
+    <t>WISCONSIN</t>
+  </si>
+  <si>
+    <t>EAST CAROLINA</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>VIRGINIA MILITARY INSTITUTE</t>
+  </si>
+  <si>
+    <t>IOWA STATE</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI STATE</t>
+  </si>
+  <si>
+    <t>ARKANSAS STATE</t>
+  </si>
+  <si>
+    <t>WESTERN MICHIGAN</t>
+  </si>
+  <si>
+    <t>TOLEDO</t>
+  </si>
+  <si>
+    <t>PRAIRIE VIEW A&amp;M</t>
+  </si>
+  <si>
+    <t>ROBERT MORRIS - PA</t>
+  </si>
+  <si>
+    <t>TULSA</t>
+  </si>
+  <si>
+    <t>GEORGIA SOUTHERN</t>
+  </si>
+  <si>
+    <t>BAYLOR</t>
+  </si>
+  <si>
+    <t>EASTERN KENTUCKY</t>
+  </si>
+  <si>
+    <t>SOUTHERN METHODIST</t>
+  </si>
+  <si>
+    <t>TENNESSEE-MARTIN</t>
+  </si>
+  <si>
+    <t>ALCORN STATE</t>
+  </si>
+  <si>
+    <t>NORTH ALABAMA</t>
+  </si>
+  <si>
+    <t>TROY STATE</t>
+  </si>
+  <si>
+    <t>NORTHWESTERN STATE-LA</t>
+  </si>
+  <si>
+    <t>BOISE</t>
+  </si>
+  <si>
+    <t>WESTERN ILLINOIS</t>
+  </si>
+  <si>
+    <t>SOUTHERN MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>VILLANOVA</t>
+  </si>
+  <si>
+    <t>ARIZONA STATE</t>
+  </si>
+  <si>
+    <t>MARSHALL</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA CENTRAL</t>
+  </si>
+  <si>
+    <t>CENTRAL FLORIDA</t>
+  </si>
+  <si>
+    <t>APPALACHIAN STATE</t>
+  </si>
+  <si>
+    <t>NORTH TEXAS</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>TULANE</t>
+  </si>
+  <si>
+    <t>HOUSTON CHRISTIAN</t>
+  </si>
+  <si>
+    <t>INCARNATE WORD</t>
+  </si>
+  <si>
+    <t>FLORIDA INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>WESTERN CAROLINA</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>RUTGERS</t>
+  </si>
+  <si>
+    <t>TARLETON STATE</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>PORTLAND STATE</t>
+  </si>
+  <si>
+    <t>ALBRIGHT</t>
   </si>
   <si>
     <t>NORTHERN ILLINOIS</t>
   </si>
   <si>
-    <t>INDIANA</t>
+    <t>NORTH DAKOTA</t>
+  </si>
+  <si>
+    <t>AIR FORCE</t>
+  </si>
+  <si>
+    <t>VANDERBILT</t>
+  </si>
+  <si>
+    <t>IDAHO STATE</t>
+  </si>
+  <si>
+    <t>RHODE ISLAND</t>
+  </si>
+  <si>
+    <t>UTAH STATE</t>
   </si>
   <si>
     <t>ALABAMA-BIRMINGHAM</t>
   </si>
   <si>
-    <t>SOUTHERN CALIFORNIA</t>
-  </si>
-  <si>
-    <t>CINCINNATI</t>
-  </si>
-  <si>
-    <t>PENN STATE</t>
-  </si>
-  <si>
-    <t>AKRON</t>
-  </si>
-  <si>
-    <t>TEXAS TECH</t>
-  </si>
-  <si>
-    <t>GEORGIA</t>
+    <t>MIAMI OF OHIO</t>
+  </si>
+  <si>
+    <t>CLEMSON</t>
+  </si>
+  <si>
+    <t>GRAMBLING</t>
   </si>
   <si>
     <t>SAN JOSE STATE</t>
   </si>
   <si>
-    <t>NEW MEXICO STATE</t>
-  </si>
-  <si>
-    <t>WASHINGTON STATE</t>
-  </si>
-  <si>
-    <t>BOISE</t>
-  </si>
-  <si>
-    <t>PITTSBURGH</t>
-  </si>
-  <si>
-    <t>SAN DIEGO STATE</t>
-  </si>
-  <si>
-    <t>LOUISVILLE</t>
-  </si>
-  <si>
-    <t>MASSACHUSETTS</t>
-  </si>
-  <si>
-    <t>COLORADO STATE</t>
-  </si>
-  <si>
-    <t>WEST VIRGINIA</t>
-  </si>
-  <si>
-    <t>SOUTHERN MISSISSIPPI</t>
-  </si>
-  <si>
-    <t>HOUSTON</t>
-  </si>
-  <si>
-    <t>GEORGIA TECH</t>
-  </si>
-  <si>
-    <t>MEMPHIS</t>
-  </si>
-  <si>
-    <t>MISSOURI</t>
-  </si>
-  <si>
-    <t>GEORGIA SOUTHERN</t>
-  </si>
-  <si>
-    <t>MARYLAND</t>
-  </si>
-  <si>
-    <t>LA - MONROE</t>
-  </si>
-  <si>
-    <t>LOUISIANA STATE</t>
-  </si>
-  <si>
-    <t>SAM HOUSTON</t>
-  </si>
-  <si>
-    <t>JAMES MADISON</t>
-  </si>
-  <si>
-    <t>EASTERN MICHIGAN</t>
-  </si>
-  <si>
-    <t>NEVADA-LAS VEGAS</t>
-  </si>
-  <si>
-    <t>OKLAHOMA STATE</t>
-  </si>
-  <si>
-    <t>KANSAS</t>
-  </si>
-  <si>
-    <t>ARKANSAS</t>
-  </si>
-  <si>
-    <t>FLORIDA</t>
-  </si>
-  <si>
-    <t>WASHINGTON</t>
-  </si>
-  <si>
-    <t>MIDDLE TENNESSEE STATE</t>
-  </si>
-  <si>
-    <t>KENT STATE</t>
-  </si>
-  <si>
-    <t>WYOMING</t>
-  </si>
-  <si>
-    <t>TEXAS-EL PASO</t>
-  </si>
-  <si>
-    <t>TEMPLE</t>
-  </si>
-  <si>
-    <t>MIAMI-FL</t>
-  </si>
-  <si>
-    <t>CENTRAL FLORIDA</t>
-  </si>
-  <si>
-    <t>STANFORD</t>
-  </si>
-  <si>
-    <t>SOUTH ALABAMA</t>
-  </si>
-  <si>
-    <t>NOTRE DAME</t>
-  </si>
-  <si>
-    <t>COASTAL CAROLINA</t>
-  </si>
-  <si>
-    <t>SYRACUSE</t>
-  </si>
-  <si>
-    <t>TEXAS A&amp;M</t>
-  </si>
-  <si>
-    <t>ALABAMA</t>
-  </si>
-  <si>
-    <t>AUBURN</t>
-  </si>
-  <si>
-    <t>FLORIDA INTERNATIONAL</t>
-  </si>
-  <si>
-    <t>BOWLING GREEN</t>
-  </si>
-  <si>
-    <t>LOUISIANA</t>
-  </si>
-  <si>
-    <t>ILLINOIS</t>
-  </si>
-  <si>
-    <t>NORTHWESTERN</t>
-  </si>
-  <si>
-    <t>TEXAS CHRISTIAN</t>
-  </si>
-  <si>
-    <t>TENNESSEE</t>
-  </si>
-  <si>
-    <t>LOUISIANA TECH</t>
-  </si>
-  <si>
-    <t>MICHIGAN STATE</t>
-  </si>
-  <si>
-    <t>BOSTON COLLEGE</t>
-  </si>
-  <si>
-    <t>BUFFALO</t>
-  </si>
-  <si>
-    <t>MISSISSIPPI STATE</t>
-  </si>
-  <si>
-    <t>PURDUE</t>
-  </si>
-  <si>
-    <t>TEXAS</t>
-  </si>
-  <si>
-    <t>JACKSONVILLE STATE</t>
-  </si>
-  <si>
-    <t>VIRGINIA TECH</t>
-  </si>
-  <si>
-    <t>OLD DOMINION</t>
-  </si>
-  <si>
-    <t>NEBRASKA</t>
-  </si>
-  <si>
-    <t>CENTRAL MICHIGAN</t>
-  </si>
-  <si>
-    <t>OHIO UNIV.</t>
-  </si>
-  <si>
-    <t>TROY STATE</t>
-  </si>
-  <si>
-    <t>WISCONSIN</t>
-  </si>
-  <si>
-    <t>EAST CAROLINA</t>
-  </si>
-  <si>
-    <t>MICHIGAN</t>
-  </si>
-  <si>
-    <t>IOWA STATE</t>
-  </si>
-  <si>
-    <t>MINNESOTA</t>
-  </si>
-  <si>
-    <t>ARIZONA</t>
-  </si>
-  <si>
-    <t>MISSISSIPPI</t>
-  </si>
-  <si>
-    <t>ARKANSAS STATE</t>
-  </si>
-  <si>
-    <t>UNC - CHARLOTTE</t>
-  </si>
-  <si>
-    <t>TOLEDO</t>
-  </si>
-  <si>
-    <t>TULSA</t>
-  </si>
-  <si>
-    <t>GEORGIA STATE</t>
-  </si>
-  <si>
-    <t>BAYLOR</t>
-  </si>
-  <si>
-    <t>WESTERN KENTUCKY</t>
-  </si>
-  <si>
-    <t>OHIO STATE</t>
-  </si>
-  <si>
-    <t>WESTERN MICHIGAN</t>
-  </si>
-  <si>
-    <t>SOUTHERN METHODIST</t>
-  </si>
-  <si>
-    <t>HAWAII</t>
-  </si>
-  <si>
-    <t>ARIZONA STATE</t>
-  </si>
-  <si>
-    <t>MARSHALL</t>
-  </si>
-  <si>
-    <t>APPALACHIAN STATE</t>
-  </si>
-  <si>
-    <t>NORTH TEXAS</t>
-  </si>
-  <si>
-    <t>NEVADA</t>
-  </si>
-  <si>
-    <t>TULANE</t>
-  </si>
-  <si>
-    <t>CALIFORNIA</t>
-  </si>
-  <si>
-    <t>RUTGERS</t>
-  </si>
-  <si>
-    <t>SOUTH CAROLINA</t>
-  </si>
-  <si>
-    <t>BRIGHAM YOUNG</t>
-  </si>
-  <si>
-    <t>NORTH CAROLINA</t>
-  </si>
-  <si>
-    <t>AIR FORCE</t>
-  </si>
-  <si>
-    <t>VANDERBILT</t>
-  </si>
-  <si>
-    <t>UTAH STATE</t>
-  </si>
-  <si>
-    <t>TEXAS STATE-SAN MARCOS</t>
-  </si>
-  <si>
-    <t>MIAMI OF OHIO</t>
-  </si>
-  <si>
-    <t>CLEMSON</t>
-  </si>
-  <si>
-    <t>U.C.L.A.</t>
+    <t>FURMAN</t>
+  </si>
+  <si>
+    <t>BUCKNELL</t>
+  </si>
+  <si>
+    <t>HOLY CROSS</t>
   </si>
 </sst>
 </file>
@@ -2549,6 +2795,9 @@
       <c r="C2" t="s">
         <v>234</v>
       </c>
+      <c r="E2" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
@@ -2560,6 +2809,9 @@
       <c r="C3" t="s">
         <v>235</v>
       </c>
+      <c r="E3" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -2571,6 +2823,9 @@
       <c r="C4" t="s">
         <v>236</v>
       </c>
+      <c r="E4" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -2586,7 +2841,7 @@
         <v>463</v>
       </c>
       <c r="E5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2599,6 +2854,9 @@
       <c r="C6" t="s">
         <v>238</v>
       </c>
+      <c r="E6" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
@@ -2627,6 +2885,9 @@
       <c r="C8" t="s">
         <v>240</v>
       </c>
+      <c r="E8" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -2642,7 +2903,7 @@
         <v>465</v>
       </c>
       <c r="E9" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2659,7 +2920,7 @@
         <v>466</v>
       </c>
       <c r="E10" t="s">
-        <v>591</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2672,6 +2933,9 @@
       <c r="C11" t="s">
         <v>243</v>
       </c>
+      <c r="E11" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -2683,6 +2947,9 @@
       <c r="C12" t="s">
         <v>244</v>
       </c>
+      <c r="E12" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -2694,6 +2961,9 @@
       <c r="C13" t="s">
         <v>245</v>
       </c>
+      <c r="E13" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -2709,7 +2979,7 @@
         <v>467</v>
       </c>
       <c r="E14" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2722,6 +2992,9 @@
       <c r="C15" t="s">
         <v>247</v>
       </c>
+      <c r="E15" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -2736,6 +3009,9 @@
       <c r="D16" t="s">
         <v>468</v>
       </c>
+      <c r="E16" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
@@ -2750,6 +3026,9 @@
       <c r="D17" t="s">
         <v>249</v>
       </c>
+      <c r="E17" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
@@ -2761,6 +3040,9 @@
       <c r="C18" t="s">
         <v>250</v>
       </c>
+      <c r="E18" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
@@ -2776,7 +3058,7 @@
         <v>469</v>
       </c>
       <c r="E19" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2789,6 +3071,9 @@
       <c r="C20" t="s">
         <v>252</v>
       </c>
+      <c r="E20" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
@@ -2800,6 +3085,9 @@
       <c r="C21" t="s">
         <v>253</v>
       </c>
+      <c r="E21" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
@@ -2812,7 +3100,7 @@
         <v>254</v>
       </c>
       <c r="E22" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2829,7 +3117,7 @@
         <v>470</v>
       </c>
       <c r="E23" t="s">
-        <v>595</v>
+        <v>604</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2846,7 +3134,7 @@
         <v>471</v>
       </c>
       <c r="E24" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2863,7 +3151,7 @@
         <v>472</v>
       </c>
       <c r="E25" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2876,6 +3164,9 @@
       <c r="C26" t="s">
         <v>258</v>
       </c>
+      <c r="E26" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
@@ -2890,6 +3181,9 @@
       <c r="D27" t="s">
         <v>473</v>
       </c>
+      <c r="E27" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
@@ -2905,7 +3199,7 @@
         <v>474</v>
       </c>
       <c r="E28" t="s">
-        <v>598</v>
+        <v>609</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2919,7 +3213,7 @@
         <v>261</v>
       </c>
       <c r="E29" t="s">
-        <v>599</v>
+        <v>610</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2932,6 +3226,9 @@
       <c r="C30" t="s">
         <v>262</v>
       </c>
+      <c r="E30" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
@@ -2947,7 +3244,7 @@
         <v>475</v>
       </c>
       <c r="E31" t="s">
-        <v>600</v>
+        <v>612</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2960,6 +3257,9 @@
       <c r="C32" t="s">
         <v>264</v>
       </c>
+      <c r="E32" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
@@ -2975,7 +3275,7 @@
         <v>476</v>
       </c>
       <c r="E33" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2992,7 +3292,7 @@
         <v>477</v>
       </c>
       <c r="E34" t="s">
-        <v>602</v>
+        <v>615</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3009,7 +3309,7 @@
         <v>478</v>
       </c>
       <c r="E35" t="s">
-        <v>603</v>
+        <v>616</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3026,7 +3326,7 @@
         <v>479</v>
       </c>
       <c r="E36" t="s">
-        <v>604</v>
+        <v>617</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3039,6 +3339,9 @@
       <c r="C37" t="s">
         <v>269</v>
       </c>
+      <c r="E37" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
@@ -3053,6 +3356,9 @@
       <c r="D38" t="s">
         <v>270</v>
       </c>
+      <c r="E38" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
@@ -3064,6 +3370,9 @@
       <c r="C39" t="s">
         <v>271</v>
       </c>
+      <c r="E39" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
@@ -3079,7 +3388,7 @@
         <v>480</v>
       </c>
       <c r="E40" t="s">
-        <v>605</v>
+        <v>621</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3092,6 +3401,9 @@
       <c r="C41" t="s">
         <v>273</v>
       </c>
+      <c r="E41" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
@@ -3103,6 +3415,9 @@
       <c r="C42" t="s">
         <v>274</v>
       </c>
+      <c r="E42" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
@@ -3115,7 +3430,7 @@
         <v>275</v>
       </c>
       <c r="E43" t="s">
-        <v>606</v>
+        <v>624</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3128,6 +3443,9 @@
       <c r="C44" t="s">
         <v>276</v>
       </c>
+      <c r="E44" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45">
@@ -3143,7 +3461,7 @@
         <v>481</v>
       </c>
       <c r="E45" t="s">
-        <v>607</v>
+        <v>626</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3156,6 +3474,9 @@
       <c r="C46" t="s">
         <v>278</v>
       </c>
+      <c r="E46" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47">
@@ -3170,6 +3491,9 @@
       <c r="D47" t="s">
         <v>279</v>
       </c>
+      <c r="E47" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48">
@@ -3182,7 +3506,7 @@
         <v>280</v>
       </c>
       <c r="E48" t="s">
-        <v>608</v>
+        <v>629</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3196,7 +3520,7 @@
         <v>281</v>
       </c>
       <c r="E49" t="s">
-        <v>609</v>
+        <v>630</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3212,6 +3536,9 @@
       <c r="D50" t="s">
         <v>482</v>
       </c>
+      <c r="E50" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51">
@@ -3227,7 +3554,7 @@
         <v>483</v>
       </c>
       <c r="E51" t="s">
-        <v>610</v>
+        <v>631</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3240,6 +3567,9 @@
       <c r="C52" t="s">
         <v>284</v>
       </c>
+      <c r="E52" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53">
@@ -3255,7 +3585,7 @@
         <v>484</v>
       </c>
       <c r="E53" t="s">
-        <v>611</v>
+        <v>633</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3272,7 +3602,7 @@
         <v>485</v>
       </c>
       <c r="E54" t="s">
-        <v>612</v>
+        <v>634</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3302,6 +3632,9 @@
       <c r="C56" t="s">
         <v>288</v>
       </c>
+      <c r="E56" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57">
@@ -3314,10 +3647,10 @@
         <v>289</v>
       </c>
       <c r="D57" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="E57" t="s">
-        <v>613</v>
+        <v>636</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3331,10 +3664,10 @@
         <v>290</v>
       </c>
       <c r="D58" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E58" t="s">
-        <v>614</v>
+        <v>637</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3348,10 +3681,10 @@
         <v>291</v>
       </c>
       <c r="D59" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E59" t="s">
-        <v>615</v>
+        <v>638</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3365,7 +3698,10 @@
         <v>292</v>
       </c>
       <c r="D60" t="s">
-        <v>490</v>
+        <v>466</v>
+      </c>
+      <c r="E60" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3379,10 +3715,10 @@
         <v>293</v>
       </c>
       <c r="D61" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E61" t="s">
-        <v>616</v>
+        <v>640</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3396,10 +3732,10 @@
         <v>294</v>
       </c>
       <c r="D62" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E62" t="s">
-        <v>617</v>
+        <v>641</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3413,10 +3749,10 @@
         <v>295</v>
       </c>
       <c r="D63" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E63" t="s">
-        <v>618</v>
+        <v>642</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3430,10 +3766,10 @@
         <v>296</v>
       </c>
       <c r="D64" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E64" t="s">
-        <v>619</v>
+        <v>643</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3446,6 +3782,9 @@
       <c r="C65" t="s">
         <v>297</v>
       </c>
+      <c r="E65" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66">
@@ -3458,10 +3797,10 @@
         <v>298</v>
       </c>
       <c r="D66" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E66" t="s">
-        <v>620</v>
+        <v>645</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3474,6 +3813,12 @@
       <c r="C67" t="s">
         <v>299</v>
       </c>
+      <c r="D67" t="s">
+        <v>494</v>
+      </c>
+      <c r="E67" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68">
@@ -3486,7 +3831,10 @@
         <v>300</v>
       </c>
       <c r="D68" t="s">
-        <v>496</v>
+        <v>495</v>
+      </c>
+      <c r="E68" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3500,7 +3848,7 @@
         <v>301</v>
       </c>
       <c r="E69" t="s">
-        <v>621</v>
+        <v>648</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3514,7 +3862,7 @@
         <v>302</v>
       </c>
       <c r="D70" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E70" t="s">
         <v>302</v>
@@ -3530,6 +3878,9 @@
       <c r="C71" t="s">
         <v>303</v>
       </c>
+      <c r="E71" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72">
@@ -3542,7 +3893,7 @@
         <v>304</v>
       </c>
       <c r="E72" t="s">
-        <v>622</v>
+        <v>650</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3556,10 +3907,10 @@
         <v>305</v>
       </c>
       <c r="D73" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E73" t="s">
-        <v>623</v>
+        <v>651</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3573,10 +3924,10 @@
         <v>306</v>
       </c>
       <c r="D74" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E74" t="s">
-        <v>624</v>
+        <v>652</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3589,6 +3940,9 @@
       <c r="C75" t="s">
         <v>307</v>
       </c>
+      <c r="E75" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76">
@@ -3601,7 +3955,7 @@
         <v>308</v>
       </c>
       <c r="D76" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E76" t="s">
         <v>308</v>
@@ -3618,7 +3972,7 @@
         <v>309</v>
       </c>
       <c r="E77" t="s">
-        <v>625</v>
+        <v>654</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3631,6 +3985,9 @@
       <c r="C78" t="s">
         <v>310</v>
       </c>
+      <c r="E78" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79">
@@ -3643,10 +4000,10 @@
         <v>311</v>
       </c>
       <c r="D79" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E79" t="s">
-        <v>626</v>
+        <v>656</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3659,6 +4016,9 @@
       <c r="C80" t="s">
         <v>312</v>
       </c>
+      <c r="E80" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81">
@@ -3671,7 +4031,7 @@
         <v>313</v>
       </c>
       <c r="E81" t="s">
-        <v>627</v>
+        <v>658</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3685,10 +4045,10 @@
         <v>314</v>
       </c>
       <c r="D82" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E82" t="s">
-        <v>628</v>
+        <v>659</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3702,10 +4062,10 @@
         <v>315</v>
       </c>
       <c r="D83" t="s">
-        <v>503</v>
+        <v>466</v>
       </c>
       <c r="E83" t="s">
-        <v>629</v>
+        <v>660</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3718,6 +4078,9 @@
       <c r="C84" t="s">
         <v>316</v>
       </c>
+      <c r="E84" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85">
@@ -3729,6 +4092,12 @@
       <c r="C85" t="s">
         <v>317</v>
       </c>
+      <c r="D85" t="s">
+        <v>502</v>
+      </c>
+      <c r="E85" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86">
@@ -3740,6 +4109,12 @@
       <c r="C86" t="s">
         <v>318</v>
       </c>
+      <c r="D86" t="s">
+        <v>503</v>
+      </c>
+      <c r="E86" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87">
@@ -3751,6 +4126,9 @@
       <c r="C87" t="s">
         <v>319</v>
       </c>
+      <c r="E87" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88">
@@ -3762,6 +4140,9 @@
       <c r="C88" t="s">
         <v>320</v>
       </c>
+      <c r="E88" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89">
@@ -3773,6 +4154,9 @@
       <c r="C89" t="s">
         <v>321</v>
       </c>
+      <c r="E89" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90">
@@ -3784,6 +4168,9 @@
       <c r="C90" t="s">
         <v>322</v>
       </c>
+      <c r="E90" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91">
@@ -3799,7 +4186,7 @@
         <v>504</v>
       </c>
       <c r="E91" t="s">
-        <v>630</v>
+        <v>667</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -3816,7 +4203,7 @@
         <v>505</v>
       </c>
       <c r="E92" t="s">
-        <v>631</v>
+        <v>668</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -3833,7 +4220,7 @@
         <v>506</v>
       </c>
       <c r="E93" t="s">
-        <v>632</v>
+        <v>669</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3850,7 +4237,7 @@
         <v>507</v>
       </c>
       <c r="E94" t="s">
-        <v>633</v>
+        <v>670</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3867,7 +4254,7 @@
         <v>508</v>
       </c>
       <c r="E95" t="s">
-        <v>634</v>
+        <v>671</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3884,7 +4271,7 @@
         <v>509</v>
       </c>
       <c r="E96" t="s">
-        <v>635</v>
+        <v>672</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -3897,6 +4284,9 @@
       <c r="C97" t="s">
         <v>329</v>
       </c>
+      <c r="E97" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98">
@@ -3912,7 +4302,7 @@
         <v>510</v>
       </c>
       <c r="E98" t="s">
-        <v>636</v>
+        <v>674</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -3929,7 +4319,7 @@
         <v>511</v>
       </c>
       <c r="E99" t="s">
-        <v>637</v>
+        <v>675</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -3942,6 +4332,9 @@
       <c r="C100" t="s">
         <v>332</v>
       </c>
+      <c r="E100" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101">
@@ -3957,7 +4350,7 @@
         <v>512</v>
       </c>
       <c r="E101" t="s">
-        <v>638</v>
+        <v>677</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -3970,6 +4363,9 @@
       <c r="C102" t="s">
         <v>334</v>
       </c>
+      <c r="E102" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103">
@@ -3984,6 +4380,9 @@
       <c r="D103" t="s">
         <v>335</v>
       </c>
+      <c r="E103" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104">
@@ -3995,6 +4394,9 @@
       <c r="C104" t="s">
         <v>336</v>
       </c>
+      <c r="E104" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105">
@@ -4010,7 +4412,7 @@
         <v>513</v>
       </c>
       <c r="E105" t="s">
-        <v>639</v>
+        <v>681</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4024,7 +4426,10 @@
         <v>338</v>
       </c>
       <c r="D106" t="s">
-        <v>514</v>
+        <v>466</v>
+      </c>
+      <c r="E106" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4040,6 +4445,9 @@
       <c r="D107" t="s">
         <v>339</v>
       </c>
+      <c r="E107" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108">
@@ -4052,10 +4460,10 @@
         <v>340</v>
       </c>
       <c r="D108" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E108" t="s">
-        <v>640</v>
+        <v>684</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4069,10 +4477,10 @@
         <v>341</v>
       </c>
       <c r="D109" t="s">
-        <v>516</v>
+        <v>466</v>
       </c>
       <c r="E109" t="s">
-        <v>641</v>
+        <v>685</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4086,10 +4494,10 @@
         <v>342</v>
       </c>
       <c r="D110" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E110" t="s">
-        <v>642</v>
+        <v>686</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4103,7 +4511,10 @@
         <v>343</v>
       </c>
       <c r="D111" t="s">
-        <v>518</v>
+        <v>466</v>
+      </c>
+      <c r="E111" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4117,10 +4528,10 @@
         <v>344</v>
       </c>
       <c r="D112" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E112" t="s">
-        <v>643</v>
+        <v>688</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4134,10 +4545,10 @@
         <v>345</v>
       </c>
       <c r="D113" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E113" t="s">
-        <v>644</v>
+        <v>689</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4151,10 +4562,10 @@
         <v>346</v>
       </c>
       <c r="D114" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E114" t="s">
-        <v>645</v>
+        <v>690</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4168,7 +4579,7 @@
         <v>347</v>
       </c>
       <c r="E115" t="s">
-        <v>646</v>
+        <v>466</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4181,6 +4592,9 @@
       <c r="C116" t="s">
         <v>348</v>
       </c>
+      <c r="E116" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117">
@@ -4192,6 +4606,9 @@
       <c r="C117" t="s">
         <v>349</v>
       </c>
+      <c r="E117" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118">
@@ -4204,10 +4621,10 @@
         <v>350</v>
       </c>
       <c r="D118" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E118" t="s">
-        <v>647</v>
+        <v>693</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4221,10 +4638,10 @@
         <v>351</v>
       </c>
       <c r="D119" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E119" t="s">
-        <v>648</v>
+        <v>694</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4238,7 +4655,7 @@
         <v>352</v>
       </c>
       <c r="E120" t="s">
-        <v>649</v>
+        <v>695</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4251,6 +4668,9 @@
       <c r="C121" t="s">
         <v>353</v>
       </c>
+      <c r="E121" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122">
@@ -4263,10 +4683,10 @@
         <v>354</v>
       </c>
       <c r="D122" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E122" t="s">
-        <v>650</v>
+        <v>697</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4280,10 +4700,10 @@
         <v>355</v>
       </c>
       <c r="D123" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E123" t="s">
-        <v>651</v>
+        <v>698</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4296,6 +4716,9 @@
       <c r="C124" t="s">
         <v>356</v>
       </c>
+      <c r="E124" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125">
@@ -4307,6 +4730,9 @@
       <c r="C125" t="s">
         <v>357</v>
       </c>
+      <c r="E125" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126">
@@ -4319,7 +4745,10 @@
         <v>358</v>
       </c>
       <c r="D126" t="s">
-        <v>526</v>
+        <v>466</v>
+      </c>
+      <c r="E126" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4332,6 +4761,9 @@
       <c r="C127" t="s">
         <v>359</v>
       </c>
+      <c r="E127" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128">
@@ -4344,10 +4776,10 @@
         <v>360</v>
       </c>
       <c r="D128" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E128" t="s">
-        <v>652</v>
+        <v>702</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4361,10 +4793,10 @@
         <v>361</v>
       </c>
       <c r="D129" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E129" t="s">
-        <v>653</v>
+        <v>703</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4378,10 +4810,10 @@
         <v>362</v>
       </c>
       <c r="D130" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E130" t="s">
-        <v>654</v>
+        <v>704</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4395,10 +4827,10 @@
         <v>363</v>
       </c>
       <c r="D131" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E131" t="s">
-        <v>655</v>
+        <v>705</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4411,6 +4843,9 @@
       <c r="C132" t="s">
         <v>364</v>
       </c>
+      <c r="E132" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133">
@@ -4423,10 +4858,10 @@
         <v>365</v>
       </c>
       <c r="D133" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="E133" t="s">
-        <v>656</v>
+        <v>707</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4439,6 +4874,9 @@
       <c r="C134" t="s">
         <v>366</v>
       </c>
+      <c r="E134" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135">
@@ -4451,10 +4889,10 @@
         <v>367</v>
       </c>
       <c r="D135" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="E135" t="s">
-        <v>657</v>
+        <v>708</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4468,10 +4906,10 @@
         <v>368</v>
       </c>
       <c r="D136" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="E136" t="s">
-        <v>658</v>
+        <v>709</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4485,10 +4923,10 @@
         <v>369</v>
       </c>
       <c r="D137" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E137" t="s">
-        <v>659</v>
+        <v>710</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4502,10 +4940,10 @@
         <v>370</v>
       </c>
       <c r="D138" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E138" t="s">
-        <v>660</v>
+        <v>628</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4519,10 +4957,10 @@
         <v>371</v>
       </c>
       <c r="D139" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="E139" t="s">
-        <v>661</v>
+        <v>711</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4536,10 +4974,10 @@
         <v>372</v>
       </c>
       <c r="D140" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="E140" t="s">
-        <v>662</v>
+        <v>712</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4553,10 +4991,10 @@
         <v>373</v>
       </c>
       <c r="D141" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="E141" t="s">
-        <v>663</v>
+        <v>713</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -4570,10 +5008,10 @@
         <v>374</v>
       </c>
       <c r="D142" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E142" t="s">
-        <v>664</v>
+        <v>714</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -4587,7 +5025,7 @@
         <v>375</v>
       </c>
       <c r="E143" t="s">
-        <v>665</v>
+        <v>715</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -4600,6 +5038,9 @@
       <c r="C144" t="s">
         <v>376</v>
       </c>
+      <c r="E144" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145">
@@ -4612,10 +5053,10 @@
         <v>377</v>
       </c>
       <c r="D145" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E145" t="s">
-        <v>666</v>
+        <v>716</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4629,10 +5070,10 @@
         <v>378</v>
       </c>
       <c r="D146" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E146" t="s">
-        <v>667</v>
+        <v>717</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -4645,6 +5086,9 @@
       <c r="C147" t="s">
         <v>379</v>
       </c>
+      <c r="E147" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148">
@@ -4657,10 +5101,10 @@
         <v>380</v>
       </c>
       <c r="D148" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="E148" t="s">
-        <v>668</v>
+        <v>718</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -4674,10 +5118,10 @@
         <v>381</v>
       </c>
       <c r="D149" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E149" t="s">
-        <v>669</v>
+        <v>719</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -4691,10 +5135,10 @@
         <v>382</v>
       </c>
       <c r="D150" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E150" t="s">
-        <v>670</v>
+        <v>720</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -4708,10 +5152,10 @@
         <v>383</v>
       </c>
       <c r="D151" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="E151" t="s">
-        <v>671</v>
+        <v>721</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -4725,10 +5169,10 @@
         <v>384</v>
       </c>
       <c r="D152" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E152" t="s">
-        <v>672</v>
+        <v>722</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -4741,8 +5185,11 @@
       <c r="C153" t="s">
         <v>385</v>
       </c>
+      <c r="D153" t="s">
+        <v>543</v>
+      </c>
       <c r="E153" t="s">
-        <v>673</v>
+        <v>723</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -4756,10 +5203,10 @@
         <v>386</v>
       </c>
       <c r="D154" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E154" t="s">
-        <v>674</v>
+        <v>724</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -4773,10 +5220,10 @@
         <v>387</v>
       </c>
       <c r="D155" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E155" t="s">
-        <v>675</v>
+        <v>725</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -4789,6 +5236,9 @@
       <c r="C156" t="s">
         <v>388</v>
       </c>
+      <c r="E156" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="157" spans="1:5">
       <c r="A157">
@@ -4803,6 +5253,9 @@
       <c r="D157" t="s">
         <v>389</v>
       </c>
+      <c r="E157" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158">
@@ -4815,10 +5268,10 @@
         <v>390</v>
       </c>
       <c r="D158" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E158" t="s">
-        <v>676</v>
+        <v>728</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -4831,6 +5284,9 @@
       <c r="C159" t="s">
         <v>391</v>
       </c>
+      <c r="E159" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160">
@@ -4843,7 +5299,10 @@
         <v>392</v>
       </c>
       <c r="D160" t="s">
-        <v>550</v>
+        <v>466</v>
+      </c>
+      <c r="E160" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -4857,7 +5316,10 @@
         <v>393</v>
       </c>
       <c r="D161" t="s">
-        <v>551</v>
+        <v>466</v>
+      </c>
+      <c r="E161" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -4871,10 +5333,10 @@
         <v>394</v>
       </c>
       <c r="D162" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="E162" t="s">
-        <v>677</v>
+        <v>732</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -4888,7 +5350,7 @@
         <v>395</v>
       </c>
       <c r="E163" t="s">
-        <v>678</v>
+        <v>733</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -4901,6 +5363,9 @@
       <c r="C164" t="s">
         <v>396</v>
       </c>
+      <c r="E164" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="165" spans="1:5">
       <c r="A165">
@@ -4912,6 +5377,9 @@
       <c r="C165" t="s">
         <v>397</v>
       </c>
+      <c r="E165" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="166" spans="1:5">
       <c r="A166">
@@ -4924,10 +5392,10 @@
         <v>398</v>
       </c>
       <c r="D166" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="E166" t="s">
-        <v>679</v>
+        <v>735</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -4941,10 +5409,10 @@
         <v>399</v>
       </c>
       <c r="D167" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="E167" t="s">
-        <v>680</v>
+        <v>736</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -4958,10 +5426,10 @@
         <v>400</v>
       </c>
       <c r="D168" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E168" t="s">
-        <v>681</v>
+        <v>737</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -4974,6 +5442,9 @@
       <c r="C169" t="s">
         <v>401</v>
       </c>
+      <c r="E169" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="170" spans="1:5">
       <c r="A170">
@@ -4986,10 +5457,10 @@
         <v>402</v>
       </c>
       <c r="D170" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="E170" t="s">
-        <v>682</v>
+        <v>739</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5003,10 +5474,10 @@
         <v>403</v>
       </c>
       <c r="D171" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="E171" t="s">
-        <v>683</v>
+        <v>740</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5020,10 +5491,10 @@
         <v>404</v>
       </c>
       <c r="D172" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="E172" t="s">
-        <v>684</v>
+        <v>741</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5037,10 +5508,10 @@
         <v>405</v>
       </c>
       <c r="D173" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="E173" t="s">
-        <v>685</v>
+        <v>742</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5054,10 +5525,10 @@
         <v>406</v>
       </c>
       <c r="D174" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="E174" t="s">
-        <v>686</v>
+        <v>743</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5071,10 +5542,10 @@
         <v>407</v>
       </c>
       <c r="D175" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="E175" t="s">
-        <v>687</v>
+        <v>744</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5088,10 +5559,10 @@
         <v>408</v>
       </c>
       <c r="D176" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="E176" t="s">
-        <v>688</v>
+        <v>745</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5104,6 +5575,9 @@
       <c r="C177" t="s">
         <v>409</v>
       </c>
+      <c r="E177" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="178" spans="1:5">
       <c r="A178">
@@ -5115,6 +5589,9 @@
       <c r="C178" t="s">
         <v>410</v>
       </c>
+      <c r="E178" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="179" spans="1:5">
       <c r="A179">
@@ -5127,10 +5604,10 @@
         <v>411</v>
       </c>
       <c r="D179" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="E179" t="s">
-        <v>689</v>
+        <v>748</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5144,10 +5621,10 @@
         <v>412</v>
       </c>
       <c r="D180" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="E180" t="s">
-        <v>690</v>
+        <v>749</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5161,10 +5638,10 @@
         <v>413</v>
       </c>
       <c r="D181" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="E181" t="s">
-        <v>691</v>
+        <v>750</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5177,6 +5654,9 @@
       <c r="C182" t="s">
         <v>414</v>
       </c>
+      <c r="E182" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="183" spans="1:5">
       <c r="A183">
@@ -5188,6 +5668,9 @@
       <c r="C183" t="s">
         <v>415</v>
       </c>
+      <c r="E183" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="184" spans="1:5">
       <c r="A184">
@@ -5199,6 +5682,9 @@
       <c r="C184" t="s">
         <v>416</v>
       </c>
+      <c r="E184" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="185" spans="1:5">
       <c r="A185">
@@ -5210,6 +5696,9 @@
       <c r="C185" t="s">
         <v>417</v>
       </c>
+      <c r="E185" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="186" spans="1:5">
       <c r="A186">
@@ -5221,6 +5710,9 @@
       <c r="C186" t="s">
         <v>418</v>
       </c>
+      <c r="E186" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="187" spans="1:5">
       <c r="A187">
@@ -5233,7 +5725,10 @@
         <v>419</v>
       </c>
       <c r="D187" t="s">
-        <v>566</v>
+        <v>561</v>
+      </c>
+      <c r="E187" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5247,7 +5742,7 @@
         <v>420</v>
       </c>
       <c r="E188" t="s">
-        <v>692</v>
+        <v>757</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5261,10 +5756,10 @@
         <v>421</v>
       </c>
       <c r="D189" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="E189" t="s">
-        <v>693</v>
+        <v>758</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5278,7 +5773,7 @@
         <v>422</v>
       </c>
       <c r="E190" t="s">
-        <v>694</v>
+        <v>759</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -5292,10 +5787,10 @@
         <v>423</v>
       </c>
       <c r="D191" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="E191" t="s">
-        <v>695</v>
+        <v>760</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5309,10 +5804,10 @@
         <v>424</v>
       </c>
       <c r="D192" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="E192" t="s">
-        <v>696</v>
+        <v>761</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5325,6 +5820,9 @@
       <c r="C193" t="s">
         <v>425</v>
       </c>
+      <c r="E193" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194">
@@ -5337,7 +5835,7 @@
         <v>426</v>
       </c>
       <c r="D194" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E194" t="s">
         <v>426</v>
@@ -5354,10 +5852,10 @@
         <v>427</v>
       </c>
       <c r="D195" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="E195" t="s">
-        <v>697</v>
+        <v>763</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5371,10 +5869,10 @@
         <v>428</v>
       </c>
       <c r="D196" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="E196" t="s">
-        <v>698</v>
+        <v>764</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5387,6 +5885,9 @@
       <c r="C197" t="s">
         <v>429</v>
       </c>
+      <c r="E197" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="198" spans="1:5">
       <c r="A198">
@@ -5401,6 +5902,9 @@
       <c r="D198" t="s">
         <v>430</v>
       </c>
+      <c r="E198" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199">
@@ -5412,8 +5916,11 @@
       <c r="C199" t="s">
         <v>431</v>
       </c>
+      <c r="D199" t="s">
+        <v>568</v>
+      </c>
       <c r="E199" t="s">
-        <v>699</v>
+        <v>767</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -5427,10 +5934,10 @@
         <v>432</v>
       </c>
       <c r="D200" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="E200" t="s">
-        <v>700</v>
+        <v>768</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5444,10 +5951,10 @@
         <v>433</v>
       </c>
       <c r="D201" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E201" t="s">
-        <v>701</v>
+        <v>769</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -5460,6 +5967,9 @@
       <c r="C202" t="s">
         <v>434</v>
       </c>
+      <c r="E202" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203">
@@ -5472,10 +5982,10 @@
         <v>435</v>
       </c>
       <c r="D203" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E203" t="s">
-        <v>702</v>
+        <v>771</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -5489,7 +5999,7 @@
         <v>436</v>
       </c>
       <c r="D204" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E204" t="s">
         <v>436</v>
@@ -5505,6 +6015,9 @@
       <c r="C205" t="s">
         <v>437</v>
       </c>
+      <c r="E205" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="206" spans="1:5">
       <c r="A206">
@@ -5516,6 +6029,9 @@
       <c r="C206" t="s">
         <v>438</v>
       </c>
+      <c r="E206" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="207" spans="1:5">
       <c r="A207">
@@ -5528,7 +6044,10 @@
         <v>439</v>
       </c>
       <c r="D207" t="s">
-        <v>577</v>
+        <v>573</v>
+      </c>
+      <c r="E207" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -5541,6 +6060,9 @@
       <c r="C208" t="s">
         <v>440</v>
       </c>
+      <c r="E208" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="209" spans="1:5">
       <c r="A209">
@@ -5553,10 +6075,10 @@
         <v>441</v>
       </c>
       <c r="D209" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E209" t="s">
-        <v>703</v>
+        <v>776</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -5570,10 +6092,10 @@
         <v>442</v>
       </c>
       <c r="D210" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="E210" t="s">
-        <v>704</v>
+        <v>777</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -5586,6 +6108,9 @@
       <c r="C211" t="s">
         <v>443</v>
       </c>
+      <c r="E211" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212">
@@ -5598,10 +6123,10 @@
         <v>444</v>
       </c>
       <c r="D212" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="E212" t="s">
-        <v>705</v>
+        <v>779</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -5614,6 +6139,9 @@
       <c r="C213" t="s">
         <v>445</v>
       </c>
+      <c r="E213" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="214" spans="1:5">
       <c r="A214">
@@ -5626,7 +6154,7 @@
         <v>446</v>
       </c>
       <c r="E214" t="s">
-        <v>706</v>
+        <v>781</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -5639,6 +6167,9 @@
       <c r="C215" t="s">
         <v>447</v>
       </c>
+      <c r="E215" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="216" spans="1:5">
       <c r="A216">
@@ -5651,7 +6182,7 @@
         <v>448</v>
       </c>
       <c r="E216" t="s">
-        <v>707</v>
+        <v>783</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -5665,10 +6196,10 @@
         <v>449</v>
       </c>
       <c r="D217" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E217" t="s">
-        <v>708</v>
+        <v>784</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -5682,10 +6213,10 @@
         <v>450</v>
       </c>
       <c r="D218" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E218" t="s">
-        <v>709</v>
+        <v>785</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -5699,7 +6230,7 @@
         <v>451</v>
       </c>
       <c r="E219" t="s">
-        <v>710</v>
+        <v>786</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -5712,6 +6243,9 @@
       <c r="C220" t="s">
         <v>452</v>
       </c>
+      <c r="E220" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="221" spans="1:5">
       <c r="A221">
@@ -5724,10 +6258,10 @@
         <v>453</v>
       </c>
       <c r="D221" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E221" t="s">
-        <v>711</v>
+        <v>788</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -5743,6 +6277,9 @@
       <c r="D222" t="s">
         <v>454</v>
       </c>
+      <c r="E222" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="223" spans="1:5">
       <c r="A223">
@@ -5755,10 +6292,10 @@
         <v>455</v>
       </c>
       <c r="D223" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E223" t="s">
-        <v>712</v>
+        <v>790</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -5772,10 +6309,10 @@
         <v>456</v>
       </c>
       <c r="D224" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E224" t="s">
-        <v>713</v>
+        <v>791</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -5788,6 +6325,9 @@
       <c r="C225" t="s">
         <v>457</v>
       </c>
+      <c r="E225" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="226" spans="1:5">
       <c r="A226">
@@ -5800,7 +6340,10 @@
         <v>458</v>
       </c>
       <c r="D226" t="s">
-        <v>586</v>
+        <v>582</v>
+      </c>
+      <c r="E226" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -5813,6 +6356,9 @@
       <c r="C227" t="s">
         <v>459</v>
       </c>
+      <c r="E227" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="228" spans="1:5">
       <c r="A228">
@@ -5825,7 +6371,7 @@
         <v>460</v>
       </c>
       <c r="E228" t="s">
-        <v>714</v>
+        <v>795</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -5839,7 +6385,7 @@
         <v>461</v>
       </c>
       <c r="D229" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E229" t="s">
         <v>461</v>
@@ -5854,6 +6400,9 @@
       </c>
       <c r="C230" t="s">
         <v>462</v>
+      </c>
+      <c r="E230" t="s">
+        <v>796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes to combine_merge and this fixed combine_stats xxxx issue
</commit_message>
<xml_diff>
--- a/data/merge.xlsx
+++ b/data/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="701">
   <si>
     <t>Index</t>
   </si>
@@ -1351,118 +1351,121 @@
     <t>COLG</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Penn St</t>
+  </si>
+  <si>
+    <t>Wash State</t>
+  </si>
+  <si>
+    <t>Bowling Grn</t>
+  </si>
+  <si>
+    <t>GA Tech</t>
+  </si>
+  <si>
+    <t>James Mad</t>
+  </si>
+  <si>
+    <t>Central Mich</t>
+  </si>
+  <si>
+    <t>Middle Tenn</t>
+  </si>
+  <si>
+    <t>S Carolina</t>
+  </si>
+  <si>
+    <t>Kent St</t>
+  </si>
+  <si>
+    <t>Fla Atlantic</t>
+  </si>
+  <si>
+    <t>TX Christian</t>
+  </si>
+  <si>
+    <t>Ohio St</t>
+  </si>
+  <si>
+    <t>S Mississippi</t>
+  </si>
+  <si>
+    <t>Miami (OH)</t>
+  </si>
+  <si>
+    <t>Boston Col</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
     <t>Connecticut</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Penn St</t>
-  </si>
-  <si>
-    <t>TX Christian</t>
-  </si>
-  <si>
-    <t>Wash State</t>
-  </si>
-  <si>
-    <t>Bowling Grn</t>
+    <t>E Carolina</t>
+  </si>
+  <si>
+    <t>VA Tech</t>
+  </si>
+  <si>
+    <t>N Carolina</t>
+  </si>
+  <si>
+    <t>Iowa St</t>
+  </si>
+  <si>
+    <t>App State</t>
+  </si>
+  <si>
+    <t>S Florida</t>
   </si>
   <si>
     <t>Miss State</t>
   </si>
   <si>
-    <t>GA Tech</t>
-  </si>
-  <si>
-    <t>James Mad</t>
-  </si>
-  <si>
-    <t>Central Mich</t>
-  </si>
-  <si>
-    <t>Middle Tenn</t>
-  </si>
-  <si>
-    <t>S Carolina</t>
-  </si>
-  <si>
-    <t>Kent St</t>
-  </si>
-  <si>
-    <t>Fla Atlantic</t>
-  </si>
-  <si>
-    <t>Ohio St</t>
-  </si>
-  <si>
-    <t>S Mississippi</t>
-  </si>
-  <si>
-    <t>Miami (OH)</t>
-  </si>
-  <si>
-    <t>Boston Col</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>E Carolina</t>
+    <t>Utah St</t>
+  </si>
+  <si>
+    <t>W Kentucky</t>
+  </si>
+  <si>
+    <t>LA Tech</t>
+  </si>
+  <si>
+    <t>U Mass</t>
+  </si>
+  <si>
+    <t>N Mex State</t>
+  </si>
+  <si>
+    <t>S Methodist</t>
+  </si>
+  <si>
+    <t>S Alabama</t>
+  </si>
+  <si>
+    <t>Ball St</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>TX El Paso</t>
+  </si>
+  <si>
+    <t>W Virginia</t>
+  </si>
+  <si>
+    <t>Jksnville St</t>
   </si>
   <si>
     <t>Sam Hous St</t>
-  </si>
-  <si>
-    <t>VA Tech</t>
-  </si>
-  <si>
-    <t>N Carolina</t>
-  </si>
-  <si>
-    <t>Iowa St</t>
-  </si>
-  <si>
-    <t>App State</t>
-  </si>
-  <si>
-    <t>S Florida</t>
-  </si>
-  <si>
-    <t>Utah St</t>
-  </si>
-  <si>
-    <t>W Kentucky</t>
-  </si>
-  <si>
-    <t>LA Tech</t>
-  </si>
-  <si>
-    <t>U Mass</t>
-  </si>
-  <si>
-    <t>N Mex State</t>
-  </si>
-  <si>
-    <t>S Methodist</t>
-  </si>
-  <si>
-    <t>S Alabama</t>
-  </si>
-  <si>
-    <t>TX El Paso</t>
-  </si>
-  <si>
-    <t>Ball St</t>
-  </si>
-  <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
-    <t>W Virginia</t>
-  </si>
-  <si>
-    <t>Jksnville St</t>
   </si>
   <si>
     <t>Florida Intl</t>
@@ -2508,7 +2511,7 @@
         <v>445</v>
       </c>
       <c r="E2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2525,7 +2528,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2542,7 +2545,7 @@
         <v>446</v>
       </c>
       <c r="E4" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2556,10 +2559,10 @@
         <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>445</v>
       </c>
       <c r="E5" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2573,10 +2576,10 @@
         <v>237</v>
       </c>
       <c r="D6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E6" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2593,7 +2596,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2607,10 +2610,10 @@
         <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>445</v>
       </c>
       <c r="E8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2627,7 +2630,7 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2641,10 +2644,10 @@
         <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E10" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2661,7 +2664,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2678,7 +2681,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2692,10 +2695,10 @@
         <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E13" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2712,7 +2715,7 @@
         <v>446</v>
       </c>
       <c r="E14" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2726,10 +2729,10 @@
         <v>246</v>
       </c>
       <c r="D15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E15" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2746,7 +2749,7 @@
         <v>447</v>
       </c>
       <c r="E16" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2760,10 +2763,10 @@
         <v>248</v>
       </c>
       <c r="D17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E17" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2780,7 +2783,7 @@
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2797,7 +2800,7 @@
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2814,7 +2817,7 @@
         <v>446</v>
       </c>
       <c r="E20" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2845,10 +2848,10 @@
         <v>253</v>
       </c>
       <c r="D22" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E22" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2865,7 +2868,7 @@
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2882,7 +2885,7 @@
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2899,7 +2902,7 @@
         <v>446</v>
       </c>
       <c r="E25" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2916,7 +2919,7 @@
         <v>446</v>
       </c>
       <c r="E26" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2930,10 +2933,10 @@
         <v>258</v>
       </c>
       <c r="D27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E27" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2950,7 +2953,7 @@
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2964,10 +2967,10 @@
         <v>260</v>
       </c>
       <c r="D29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E29" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2984,7 +2987,7 @@
         <v>446</v>
       </c>
       <c r="E30" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3001,7 +3004,7 @@
         <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3015,10 +3018,10 @@
         <v>262</v>
       </c>
       <c r="D32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E32" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3032,10 +3035,10 @@
         <v>263</v>
       </c>
       <c r="D33" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E33" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3052,7 +3055,7 @@
         <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3069,7 +3072,7 @@
         <v>38</v>
       </c>
       <c r="E35" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3086,7 +3089,7 @@
         <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3103,7 +3106,7 @@
         <v>446</v>
       </c>
       <c r="E37" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3120,7 +3123,7 @@
         <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3137,7 +3140,7 @@
         <v>42</v>
       </c>
       <c r="E39" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3154,7 +3157,7 @@
         <v>446</v>
       </c>
       <c r="E40" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3171,7 +3174,7 @@
         <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3188,7 +3191,7 @@
         <v>45</v>
       </c>
       <c r="E42" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3205,7 +3208,7 @@
         <v>446</v>
       </c>
       <c r="E43" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3222,7 +3225,7 @@
         <v>47</v>
       </c>
       <c r="E44" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3236,10 +3239,10 @@
         <v>273</v>
       </c>
       <c r="D45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E45" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3253,10 +3256,10 @@
         <v>274</v>
       </c>
       <c r="D46" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E46" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3270,10 +3273,10 @@
         <v>275</v>
       </c>
       <c r="D47" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E47" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -3290,7 +3293,7 @@
         <v>51</v>
       </c>
       <c r="E48" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3304,10 +3307,10 @@
         <v>277</v>
       </c>
       <c r="D49" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E49" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3324,7 +3327,7 @@
         <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3338,10 +3341,10 @@
         <v>279</v>
       </c>
       <c r="D51" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E51" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3355,7 +3358,7 @@
         <v>280</v>
       </c>
       <c r="D52" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E52" t="s">
         <v>280</v>
@@ -3372,10 +3375,10 @@
         <v>281</v>
       </c>
       <c r="D53" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E53" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3389,10 +3392,10 @@
         <v>282</v>
       </c>
       <c r="D54" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E54" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3409,7 +3412,7 @@
         <v>58</v>
       </c>
       <c r="E55" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3426,7 +3429,7 @@
         <v>59</v>
       </c>
       <c r="E56" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3443,7 +3446,7 @@
         <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3460,7 +3463,7 @@
         <v>446</v>
       </c>
       <c r="E58" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3474,10 +3477,10 @@
         <v>286</v>
       </c>
       <c r="D59" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E59" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3491,10 +3494,10 @@
         <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E60" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3511,7 +3514,7 @@
         <v>64</v>
       </c>
       <c r="E61" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3528,7 +3531,7 @@
         <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3545,7 +3548,7 @@
         <v>66</v>
       </c>
       <c r="E63" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3562,7 +3565,7 @@
         <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3579,7 +3582,7 @@
         <v>68</v>
       </c>
       <c r="E65" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3593,10 +3596,10 @@
         <v>290</v>
       </c>
       <c r="D66" t="s">
-        <v>100</v>
+        <v>445</v>
       </c>
       <c r="E66" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3610,10 +3613,10 @@
         <v>291</v>
       </c>
       <c r="D67" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E67" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3630,7 +3633,7 @@
         <v>71</v>
       </c>
       <c r="E68" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3644,10 +3647,10 @@
         <v>293</v>
       </c>
       <c r="D69" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E69" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3664,7 +3667,7 @@
         <v>73</v>
       </c>
       <c r="E70" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3678,10 +3681,10 @@
         <v>295</v>
       </c>
       <c r="D71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E71" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3695,10 +3698,10 @@
         <v>296</v>
       </c>
       <c r="D72" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E72" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3715,7 +3718,7 @@
         <v>76</v>
       </c>
       <c r="E73" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3729,10 +3732,10 @@
         <v>298</v>
       </c>
       <c r="D74" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E74" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3749,7 +3752,7 @@
         <v>446</v>
       </c>
       <c r="E75" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3766,7 +3769,7 @@
         <v>446</v>
       </c>
       <c r="E76" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3780,10 +3783,10 @@
         <v>301</v>
       </c>
       <c r="D77" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E77" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3800,7 +3803,7 @@
         <v>446</v>
       </c>
       <c r="E78" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3817,7 +3820,7 @@
         <v>446</v>
       </c>
       <c r="E79" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3834,7 +3837,7 @@
         <v>446</v>
       </c>
       <c r="E80" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3851,7 +3854,7 @@
         <v>84</v>
       </c>
       <c r="E81" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3868,7 +3871,7 @@
         <v>85</v>
       </c>
       <c r="E82" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3882,10 +3885,10 @@
         <v>307</v>
       </c>
       <c r="D83" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E83" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3899,10 +3902,10 @@
         <v>308</v>
       </c>
       <c r="D84" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E84" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3916,10 +3919,10 @@
         <v>309</v>
       </c>
       <c r="D85" t="s">
-        <v>138</v>
+        <v>445</v>
       </c>
       <c r="E85" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -3936,7 +3939,7 @@
         <v>446</v>
       </c>
       <c r="E86" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -3950,10 +3953,10 @@
         <v>90</v>
       </c>
       <c r="D87" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E87" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3967,10 +3970,10 @@
         <v>91</v>
       </c>
       <c r="D88" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="E88" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -3984,10 +3987,10 @@
         <v>311</v>
       </c>
       <c r="D89" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E89" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4001,10 +4004,10 @@
         <v>312</v>
       </c>
       <c r="D90" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E90" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4018,10 +4021,10 @@
         <v>313</v>
       </c>
       <c r="D91" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E91" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4035,10 +4038,10 @@
         <v>314</v>
       </c>
       <c r="D92" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E92" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4052,10 +4055,10 @@
         <v>315</v>
       </c>
       <c r="D93" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E93" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -4069,10 +4072,10 @@
         <v>316</v>
       </c>
       <c r="D94" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E94" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4089,7 +4092,7 @@
         <v>98</v>
       </c>
       <c r="E95" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4106,7 +4109,7 @@
         <v>446</v>
       </c>
       <c r="E96" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4123,7 +4126,7 @@
         <v>100</v>
       </c>
       <c r="E97" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4140,7 +4143,7 @@
         <v>101</v>
       </c>
       <c r="E98" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4154,10 +4157,10 @@
         <v>102</v>
       </c>
       <c r="D99" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E99" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4174,7 +4177,7 @@
         <v>446</v>
       </c>
       <c r="E100" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4188,10 +4191,10 @@
         <v>322</v>
       </c>
       <c r="D101" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E101" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4208,7 +4211,7 @@
         <v>105</v>
       </c>
       <c r="E102" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4225,7 +4228,7 @@
         <v>106</v>
       </c>
       <c r="E103" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -4259,7 +4262,7 @@
         <v>108</v>
       </c>
       <c r="E105" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4273,10 +4276,10 @@
         <v>327</v>
       </c>
       <c r="D106" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E106" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4310,7 +4313,7 @@
         <v>446</v>
       </c>
       <c r="E108" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4324,10 +4327,10 @@
         <v>330</v>
       </c>
       <c r="D109" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E109" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4341,10 +4344,10 @@
         <v>331</v>
       </c>
       <c r="D110" t="s">
-        <v>445</v>
+        <v>463</v>
       </c>
       <c r="E110" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4361,7 +4364,7 @@
         <v>446</v>
       </c>
       <c r="E111" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4378,7 +4381,7 @@
         <v>115</v>
       </c>
       <c r="E112" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4395,7 +4398,7 @@
         <v>464</v>
       </c>
       <c r="E113" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4412,7 +4415,7 @@
         <v>117</v>
       </c>
       <c r="E114" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4429,7 +4432,7 @@
         <v>118</v>
       </c>
       <c r="E115" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4446,7 +4449,7 @@
         <v>119</v>
       </c>
       <c r="E116" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4463,7 +4466,7 @@
         <v>446</v>
       </c>
       <c r="E117" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4480,7 +4483,7 @@
         <v>121</v>
       </c>
       <c r="E118" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4497,7 +4500,7 @@
         <v>122</v>
       </c>
       <c r="E119" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4511,10 +4514,10 @@
         <v>341</v>
       </c>
       <c r="D120" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E120" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4531,7 +4534,7 @@
         <v>446</v>
       </c>
       <c r="E121" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4548,7 +4551,7 @@
         <v>125</v>
       </c>
       <c r="E122" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4562,10 +4565,10 @@
         <v>344</v>
       </c>
       <c r="D123" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="E123" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4582,7 +4585,7 @@
         <v>127</v>
       </c>
       <c r="E124" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4599,7 +4602,7 @@
         <v>128</v>
       </c>
       <c r="E125" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4616,7 +4619,7 @@
         <v>129</v>
       </c>
       <c r="E126" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4630,10 +4633,10 @@
         <v>348</v>
       </c>
       <c r="D127" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E127" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -4647,10 +4650,10 @@
         <v>349</v>
       </c>
       <c r="D128" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E128" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4667,7 +4670,7 @@
         <v>446</v>
       </c>
       <c r="E129" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4684,7 +4687,7 @@
         <v>133</v>
       </c>
       <c r="E130" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4701,7 +4704,7 @@
         <v>134</v>
       </c>
       <c r="E131" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4718,7 +4721,7 @@
         <v>135</v>
       </c>
       <c r="E132" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -4735,7 +4738,7 @@
         <v>136</v>
       </c>
       <c r="E133" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4752,7 +4755,7 @@
         <v>446</v>
       </c>
       <c r="E134" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -4769,7 +4772,7 @@
         <v>138</v>
       </c>
       <c r="E135" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4786,7 +4789,7 @@
         <v>139</v>
       </c>
       <c r="E136" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4800,10 +4803,10 @@
         <v>358</v>
       </c>
       <c r="D137" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E137" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4817,10 +4820,10 @@
         <v>359</v>
       </c>
       <c r="D138" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E138" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4837,7 +4840,7 @@
         <v>446</v>
       </c>
       <c r="E139" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4854,7 +4857,7 @@
         <v>143</v>
       </c>
       <c r="E140" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4868,10 +4871,10 @@
         <v>361</v>
       </c>
       <c r="D141" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E141" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -4888,7 +4891,7 @@
         <v>145</v>
       </c>
       <c r="E142" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -4905,7 +4908,7 @@
         <v>446</v>
       </c>
       <c r="E143" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -4922,7 +4925,7 @@
         <v>446</v>
       </c>
       <c r="E144" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -4936,10 +4939,10 @@
         <v>365</v>
       </c>
       <c r="D145" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E145" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4953,10 +4956,10 @@
         <v>366</v>
       </c>
       <c r="D146" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E146" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -4970,10 +4973,10 @@
         <v>367</v>
       </c>
       <c r="D147" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E147" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -4990,7 +4993,7 @@
         <v>151</v>
       </c>
       <c r="E148" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5007,7 +5010,7 @@
         <v>446</v>
       </c>
       <c r="E149" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5024,7 +5027,7 @@
         <v>153</v>
       </c>
       <c r="E150" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5038,10 +5041,10 @@
         <v>371</v>
       </c>
       <c r="D151" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E151" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5058,7 +5061,7 @@
         <v>155</v>
       </c>
       <c r="E152" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5092,7 +5095,7 @@
         <v>446</v>
       </c>
       <c r="E154" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5106,10 +5109,10 @@
         <v>375</v>
       </c>
       <c r="D155" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E155" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5126,7 +5129,7 @@
         <v>159</v>
       </c>
       <c r="E156" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5140,10 +5143,10 @@
         <v>377</v>
       </c>
       <c r="D157" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E157" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5160,7 +5163,7 @@
         <v>161</v>
       </c>
       <c r="E158" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5174,10 +5177,10 @@
         <v>379</v>
       </c>
       <c r="D159" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E159" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5191,10 +5194,10 @@
         <v>380</v>
       </c>
       <c r="D160" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E160" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -5228,7 +5231,7 @@
         <v>446</v>
       </c>
       <c r="E162" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5242,10 +5245,10 @@
         <v>383</v>
       </c>
       <c r="D163" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E163" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5259,10 +5262,10 @@
         <v>384</v>
       </c>
       <c r="D164" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="E164" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5279,7 +5282,7 @@
         <v>168</v>
       </c>
       <c r="E165" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5296,7 +5299,7 @@
         <v>169</v>
       </c>
       <c r="E166" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5310,10 +5313,10 @@
         <v>387</v>
       </c>
       <c r="D167" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E167" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5327,10 +5330,10 @@
         <v>388</v>
       </c>
       <c r="D168" t="s">
-        <v>451</v>
+        <v>470</v>
       </c>
       <c r="E168" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5347,7 +5350,7 @@
         <v>172</v>
       </c>
       <c r="E169" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -5364,7 +5367,7 @@
         <v>446</v>
       </c>
       <c r="E170" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5378,10 +5381,10 @@
         <v>391</v>
       </c>
       <c r="D171" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E171" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5398,7 +5401,7 @@
         <v>446</v>
       </c>
       <c r="E172" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5415,7 +5418,7 @@
         <v>176</v>
       </c>
       <c r="E173" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5432,7 +5435,7 @@
         <v>446</v>
       </c>
       <c r="E174" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5446,10 +5449,10 @@
         <v>395</v>
       </c>
       <c r="D175" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E175" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5466,7 +5469,7 @@
         <v>446</v>
       </c>
       <c r="E176" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5483,7 +5486,7 @@
         <v>471</v>
       </c>
       <c r="E177" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -5500,7 +5503,7 @@
         <v>446</v>
       </c>
       <c r="E178" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -5517,7 +5520,7 @@
         <v>446</v>
       </c>
       <c r="E179" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5534,7 +5537,7 @@
         <v>183</v>
       </c>
       <c r="E180" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5568,7 +5571,7 @@
         <v>185</v>
       </c>
       <c r="E182" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5585,7 +5588,7 @@
         <v>186</v>
       </c>
       <c r="E183" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -5602,7 +5605,7 @@
         <v>472</v>
       </c>
       <c r="E184" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -5619,7 +5622,7 @@
         <v>473</v>
       </c>
       <c r="E185" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -5636,7 +5639,7 @@
         <v>189</v>
       </c>
       <c r="E186" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -5653,7 +5656,7 @@
         <v>474</v>
       </c>
       <c r="E187" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5670,7 +5673,7 @@
         <v>475</v>
       </c>
       <c r="E188" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5687,7 +5690,7 @@
         <v>192</v>
       </c>
       <c r="E189" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5704,7 +5707,7 @@
         <v>193</v>
       </c>
       <c r="E190" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -5721,7 +5724,7 @@
         <v>194</v>
       </c>
       <c r="E191" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5738,7 +5741,7 @@
         <v>476</v>
       </c>
       <c r="E192" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5755,7 +5758,7 @@
         <v>446</v>
       </c>
       <c r="E193" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -5772,7 +5775,7 @@
         <v>477</v>
       </c>
       <c r="E194" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -5789,7 +5792,7 @@
         <v>446</v>
       </c>
       <c r="E195" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5806,7 +5809,7 @@
         <v>199</v>
       </c>
       <c r="E196" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5823,7 +5826,7 @@
         <v>446</v>
       </c>
       <c r="E197" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -5837,10 +5840,10 @@
         <v>417</v>
       </c>
       <c r="D198" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E198" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -5854,10 +5857,10 @@
         <v>418</v>
       </c>
       <c r="D199" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="E199" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -5874,7 +5877,7 @@
         <v>446</v>
       </c>
       <c r="E200" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5891,7 +5894,7 @@
         <v>204</v>
       </c>
       <c r="E201" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -5905,10 +5908,10 @@
         <v>420</v>
       </c>
       <c r="D202" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E202" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -5925,7 +5928,7 @@
         <v>446</v>
       </c>
       <c r="E203" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -5942,7 +5945,7 @@
         <v>207</v>
       </c>
       <c r="E204" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -5959,7 +5962,7 @@
         <v>208</v>
       </c>
       <c r="E205" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -5973,10 +5976,10 @@
         <v>424</v>
       </c>
       <c r="D206" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E206" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -5993,7 +5996,7 @@
         <v>210</v>
       </c>
       <c r="E207" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -6007,10 +6010,10 @@
         <v>211</v>
       </c>
       <c r="D208" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E208" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6027,7 +6030,7 @@
         <v>481</v>
       </c>
       <c r="E209" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6044,7 +6047,7 @@
         <v>213</v>
       </c>
       <c r="E210" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6058,10 +6061,10 @@
         <v>428</v>
       </c>
       <c r="D211" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E211" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -6078,7 +6081,7 @@
         <v>482</v>
       </c>
       <c r="E212" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6095,7 +6098,7 @@
         <v>216</v>
       </c>
       <c r="E213" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6112,7 +6115,7 @@
         <v>217</v>
       </c>
       <c r="E214" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -6129,7 +6132,7 @@
         <v>218</v>
       </c>
       <c r="E215" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6146,7 +6149,7 @@
         <v>219</v>
       </c>
       <c r="E216" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6163,7 +6166,7 @@
         <v>446</v>
       </c>
       <c r="E217" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6180,7 +6183,7 @@
         <v>446</v>
       </c>
       <c r="E218" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6194,10 +6197,10 @@
         <v>435</v>
       </c>
       <c r="D219" t="s">
-        <v>465</v>
+        <v>483</v>
       </c>
       <c r="E219" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -6214,7 +6217,7 @@
         <v>223</v>
       </c>
       <c r="E220" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -6231,7 +6234,7 @@
         <v>224</v>
       </c>
       <c r="E221" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6248,7 +6251,7 @@
         <v>446</v>
       </c>
       <c r="E222" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -6265,7 +6268,7 @@
         <v>226</v>
       </c>
       <c r="E223" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -6282,7 +6285,7 @@
         <v>446</v>
       </c>
       <c r="E224" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6296,10 +6299,10 @@
         <v>441</v>
       </c>
       <c r="D225" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E225" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -6313,10 +6316,10 @@
         <v>229</v>
       </c>
       <c r="D226" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E226" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6333,7 +6336,7 @@
         <v>230</v>
       </c>
       <c r="E227" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -6350,7 +6353,7 @@
         <v>231</v>
       </c>
       <c r="E228" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6364,10 +6367,10 @@
         <v>444</v>
       </c>
       <c r="D229" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E229" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>